<commit_message>
Refactor the NIST Statistical Tests: change the return value of tests
</commit_message>
<xml_diff>
--- a/results/Random Sequences Results.xlsx
+++ b/results/Random Sequences Results.xlsx
@@ -528,26 +528,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFF66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF66"/>
         <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFF66"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF99FF99"/>
         <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3333"/>
-        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -567,7 +567,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -591,6 +591,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -621,7 +627,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -629,31 +659,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -662,14 +668,44 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="yellow" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="red" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -741,56 +777,39 @@
   <dimension ref="B4:DQ96"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E51" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="BX54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="F54" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
-      <selection pane="topRight" activeCell="BX51" activeCellId="0" sqref="BX51"/>
+      <selection pane="topRight" activeCell="F51" activeCellId="0" sqref="F51"/>
       <selection pane="bottomLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
-      <selection pane="bottomRight" activeCell="CI82" activeCellId="0" sqref="CI82"/>
+      <selection pane="bottomRight" activeCell="H59" activeCellId="0" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.0357142857143"/>
-    <col collapsed="false" hidden="false" max="22" min="14" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="28" min="24" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="34" min="30" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="40" min="36" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="46" min="42" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="52" min="48" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="58" min="54" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="64" min="60" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="70" min="66" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="76" min="73" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="82" min="78" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="23.8418367346939"/>
-    <col collapsed="false" hidden="false" max="85" min="85" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="87" min="87" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="15.6428571428571"/>
-    <col collapsed="false" hidden="false" max="90" min="89" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="92" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="85" min="85" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="87" min="87" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="21.1938775510204"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12546,6 +12565,15 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G54:CJ96">
+    <cfRule type="cellIs" priority="2" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>6</formula>
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Start writing BookStack part
</commit_message>
<xml_diff>
--- a/results/Random Sequences Results.xlsx
+++ b/results/Random Sequences Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="146">
   <si>
     <t>BookStackTest_8dim_16up</t>
   </si>
@@ -455,13 +455,16 @@
   </si>
   <si>
     <t xml:space="preserve">  требует проверки</t>
+  </si>
+  <si>
+    <t>сложно интерпретировать результаты, так как тест выдаёт сразу пачку результатов</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -747,7 +750,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -782,7 +784,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -958,18 +959,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:DQ94"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" topLeftCell="E51" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="CC60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="CE54" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E51" sqref="E51"/>
       <selection pane="topRight" activeCell="BT51" sqref="BT51"/>
       <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
-      <selection pane="bottomRight" activeCell="CL76" sqref="CL76"/>
+      <selection pane="bottomRight" activeCell="CF54" sqref="CF54:CJ90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="4" width="12.28515625"/>
     <col min="5" max="5" width="34.7109375" customWidth="1"/>
@@ -978,7 +979,7 @@
     <col min="85" max="1025" width="12.28515625"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:48" ht="15.75" customHeight="1">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1105,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:48" ht="15.75" customHeight="1">
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1233,7 +1234,7 @@
         <v>-100000</v>
       </c>
     </row>
-    <row r="6" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:48" ht="15.75" customHeight="1">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1359,7 +1360,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:48" ht="15.75" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1488,7 +1489,7 @@
         <v>-89000</v>
       </c>
     </row>
-    <row r="8" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:48" ht="15.75" customHeight="1">
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:48" ht="15.75" customHeight="1">
       <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>-56000</v>
       </c>
     </row>
-    <row r="10" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:48" ht="15.75" customHeight="1">
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1869,7 +1870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:48" ht="15.75" customHeight="1">
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>-51000</v>
       </c>
     </row>
-    <row r="12" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:48" ht="15.75" customHeight="1">
       <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
@@ -2012,7 +2013,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:48" ht="15.75" customHeight="1">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2028,7 +2029,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:48" ht="15.75" customHeight="1">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2044,7 +2045,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:48" ht="15.75" customHeight="1">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2060,7 +2061,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:48" ht="15.75" customHeight="1">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2076,7 +2077,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:16" ht="15.75" customHeight="1">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2092,7 +2093,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:16" ht="15.75" customHeight="1">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2108,7 +2109,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:16" ht="15.75" customHeight="1">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2124,7 +2125,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:16" ht="15.75" customHeight="1">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2140,7 +2141,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:16" ht="15.75" customHeight="1">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2156,7 +2157,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:16" ht="15.75" customHeight="1">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2172,7 +2173,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" ht="15.75" customHeight="1">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2188,7 +2189,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" ht="15.75" customHeight="1">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2204,7 +2205,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" ht="15.75" customHeight="1">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2220,7 +2221,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" ht="15.75" customHeight="1">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2236,7 +2237,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" ht="15.75" customHeight="1">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2252,7 +2253,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" ht="15.75" customHeight="1">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2268,7 +2269,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" ht="15.75" customHeight="1">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2284,7 +2285,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:16" ht="15.75" customHeight="1">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2300,7 +2301,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:16" ht="15.75" customHeight="1">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2316,7 +2317,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:16" ht="15.75" customHeight="1">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2332,7 +2333,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:116" ht="15.75" customHeight="1">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2348,7 +2349,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:116" ht="15.75" customHeight="1">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2364,7 +2365,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:116" ht="15.75" customHeight="1">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2426,7 +2427,7 @@
       <c r="BR35" s="1"/>
       <c r="BS35" s="1"/>
     </row>
-    <row r="36" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:116" ht="15.75" customHeight="1">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2488,7 +2489,7 @@
       <c r="BR36" s="1"/>
       <c r="BS36" s="1"/>
     </row>
-    <row r="37" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:116" ht="15.75" customHeight="1">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2550,7 +2551,7 @@
       <c r="BR37" s="1"/>
       <c r="BS37" s="1"/>
     </row>
-    <row r="38" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:116" ht="15.75" customHeight="1">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2618,7 +2619,7 @@
       <c r="BR38" s="1"/>
       <c r="BS38" s="1"/>
     </row>
-    <row r="39" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:116" ht="15.75" customHeight="1">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2681,7 +2682,7 @@
       <c r="BM39" s="1"/>
       <c r="BN39" s="1"/>
     </row>
-    <row r="40" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:116" ht="15.75" customHeight="1">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2744,7 +2745,7 @@
       <c r="BM40" s="1"/>
       <c r="BN40" s="1"/>
     </row>
-    <row r="41" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:116" ht="15.75" customHeight="1">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2826,7 +2827,7 @@
       <c r="CF41" s="1"/>
       <c r="CG41" s="1"/>
     </row>
-    <row r="42" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:116" ht="15.75" customHeight="1">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2887,7 +2888,7 @@
       <c r="CF42" s="1"/>
       <c r="CG42" s="1"/>
     </row>
-    <row r="43" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:116" ht="15.75" customHeight="1">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2972,7 +2973,7 @@
       <c r="CF43" s="1"/>
       <c r="CG43" s="1"/>
     </row>
-    <row r="44" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:116" ht="15.75" customHeight="1">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -3078,7 +3079,7 @@
       <c r="DA44" s="1"/>
       <c r="DB44" s="1"/>
     </row>
-    <row r="45" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:116" ht="15.75" customHeight="1">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -3184,7 +3185,7 @@
       <c r="DA45" s="1"/>
       <c r="DB45" s="1"/>
     </row>
-    <row r="46" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:116" ht="15.75" customHeight="1">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3300,7 +3301,7 @@
       <c r="DK46" s="1"/>
       <c r="DL46" s="1"/>
     </row>
-    <row r="47" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:116" ht="15.75" customHeight="1">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -3399,7 +3400,7 @@
       <c r="DK47" s="1"/>
       <c r="DL47" s="1"/>
     </row>
-    <row r="48" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:116" ht="15.75" customHeight="1">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -3499,7 +3500,7 @@
       <c r="DK48" s="1"/>
       <c r="DL48" s="1"/>
     </row>
-    <row r="49" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:121" ht="15.75" customHeight="1">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -3611,7 +3612,7 @@
       <c r="DP49" s="1"/>
       <c r="DQ49" s="1"/>
     </row>
-    <row r="50" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:121" ht="15.75" customHeight="1">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -3691,7 +3692,7 @@
       <c r="DG50" s="1"/>
       <c r="DH50" s="1"/>
     </row>
-    <row r="51" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:121" ht="15.75" customHeight="1">
       <c r="H51" s="3" t="s">
         <v>41</v>
       </c>
@@ -3755,7 +3756,7 @@
       <c r="DK51" s="1"/>
       <c r="DL51" s="1"/>
     </row>
-    <row r="52" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:121" ht="15.75" customHeight="1">
       <c r="B52" s="1" t="s">
         <v>43</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:121" ht="15.75" customHeight="1">
       <c r="C53" s="1" t="s">
         <v>63</v>
       </c>
@@ -4127,7 +4128,7 @@
       <c r="DA53" s="1"/>
       <c r="DB53" s="1"/>
     </row>
-    <row r="54" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:121" ht="15.75" customHeight="1">
       <c r="B54" s="1" t="s">
         <v>0</v>
       </c>
@@ -4335,7 +4336,9 @@
       <c r="CE54" s="7">
         <v>1</v>
       </c>
-      <c r="CF54" s="8"/>
+      <c r="CF54" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="CG54" s="8">
         <v>1</v>
       </c>
@@ -4349,7 +4352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:121" ht="15.75" customHeight="1">
       <c r="B55" s="1" t="s">
         <v>1</v>
       </c>
@@ -4547,7 +4550,9 @@
       <c r="CE55" s="7">
         <v>1</v>
       </c>
-      <c r="CF55" s="8"/>
+      <c r="CF55" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="CG55" s="8">
         <v>2</v>
       </c>
@@ -4561,7 +4566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:121" ht="15.75" customHeight="1">
       <c r="B56" s="1" t="s">
         <v>2</v>
       </c>
@@ -4761,7 +4766,9 @@
       <c r="CE56" s="7">
         <v>0</v>
       </c>
-      <c r="CF56" s="8"/>
+      <c r="CF56" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="CG56" s="8">
         <v>0</v>
       </c>
@@ -4775,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:121" ht="15.75" customHeight="1">
       <c r="B57" s="1" t="s">
         <v>0</v>
       </c>
@@ -4983,7 +4990,9 @@
       <c r="CE57" s="7">
         <v>1</v>
       </c>
-      <c r="CF57" s="8"/>
+      <c r="CF57" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="CG57" s="8">
         <v>1</v>
       </c>
@@ -4997,7 +5006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:121" ht="15.75" customHeight="1">
       <c r="B58" s="1" t="s">
         <v>3</v>
       </c>
@@ -5197,7 +5206,9 @@
       <c r="CE58" s="7">
         <v>1</v>
       </c>
-      <c r="CF58" s="8"/>
+      <c r="CF58" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="CG58" s="8">
         <v>3</v>
       </c>
@@ -5211,7 +5222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:121" ht="15.75" customHeight="1">
       <c r="B59" s="1" t="s">
         <v>4</v>
       </c>
@@ -5411,7 +5422,9 @@
       <c r="CE59" s="7">
         <v>0</v>
       </c>
-      <c r="CF59" s="8"/>
+      <c r="CF59" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="CG59" s="8">
         <v>7</v>
       </c>
@@ -5425,7 +5438,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:121" ht="15.75" customHeight="1">
       <c r="B60" s="1" t="s">
         <v>5</v>
       </c>
@@ -5633,7 +5646,9 @@
       <c r="CE60" s="7">
         <v>1</v>
       </c>
-      <c r="CF60" s="8"/>
+      <c r="CF60" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="CG60" s="8">
         <v>1</v>
       </c>
@@ -5647,7 +5662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:121" ht="15.75" customHeight="1">
       <c r="B61" s="1" t="s">
         <v>129</v>
       </c>
@@ -5847,7 +5862,9 @@
       <c r="CE61" s="7">
         <v>0</v>
       </c>
-      <c r="CF61" s="8"/>
+      <c r="CF61" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="CG61" s="8">
         <v>1</v>
       </c>
@@ -5861,7 +5878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:121" ht="15.75" customHeight="1">
       <c r="B62" s="1" t="s">
         <v>6</v>
       </c>
@@ -6069,7 +6086,9 @@
       <c r="CE62" s="7">
         <v>1</v>
       </c>
-      <c r="CF62" s="8"/>
+      <c r="CF62" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="CG62" s="8">
         <v>3</v>
       </c>
@@ -6083,7 +6102,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:121" ht="15.75" customHeight="1">
       <c r="B63" s="1" t="s">
         <v>7</v>
       </c>
@@ -6291,7 +6310,9 @@
       <c r="CE63" s="7">
         <v>1</v>
       </c>
-      <c r="CF63" s="8"/>
+      <c r="CF63" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="CG63" s="8">
         <v>0</v>
       </c>
@@ -6305,7 +6326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:121" ht="15.75" customHeight="1">
       <c r="B64" s="1" t="s">
         <v>130</v>
       </c>
@@ -6513,7 +6534,9 @@
       <c r="CE64" s="7">
         <v>1</v>
       </c>
-      <c r="CF64" s="8"/>
+      <c r="CF64" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="CG64" s="8">
         <v>4</v>
       </c>
@@ -6527,7 +6550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:89" ht="15.75" customHeight="1">
       <c r="B65" s="1" t="s">
         <v>131</v>
       </c>
@@ -6735,7 +6758,9 @@
       <c r="CE65" s="7">
         <v>0</v>
       </c>
-      <c r="CF65" s="8"/>
+      <c r="CF65" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="CG65" s="8">
         <v>2</v>
       </c>
@@ -6749,7 +6774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:89" ht="15.75" customHeight="1">
       <c r="B66" s="1" t="s">
         <v>11</v>
       </c>
@@ -6957,7 +6982,9 @@
       <c r="CE66" s="7">
         <v>2</v>
       </c>
-      <c r="CF66" s="8"/>
+      <c r="CF66" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="CG66" s="8">
         <v>1</v>
       </c>
@@ -6971,7 +6998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:89" ht="15.75" customHeight="1">
       <c r="B67" s="1" t="s">
         <v>12</v>
       </c>
@@ -7179,7 +7206,9 @@
       <c r="CE67" s="7">
         <v>2</v>
       </c>
-      <c r="CF67" s="8"/>
+      <c r="CF67" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="CG67" s="8">
         <v>1</v>
       </c>
@@ -7193,7 +7222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:89" ht="15.75" customHeight="1">
       <c r="B68" s="1" t="s">
         <v>13</v>
       </c>
@@ -7401,7 +7430,9 @@
       <c r="CE68" s="7">
         <v>0</v>
       </c>
-      <c r="CF68" s="8"/>
+      <c r="CF68" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="CG68" s="8">
         <v>4</v>
       </c>
@@ -7415,7 +7446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:89" ht="15.75" customHeight="1">
       <c r="B69" s="1" t="s">
         <v>14</v>
       </c>
@@ -7623,7 +7654,9 @@
       <c r="CE69" s="7">
         <v>0</v>
       </c>
-      <c r="CF69" s="8"/>
+      <c r="CF69" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="CG69" s="8">
         <v>3</v>
       </c>
@@ -7637,7 +7670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:89" ht="15.75" customHeight="1">
       <c r="B70" s="1" t="s">
         <v>15</v>
       </c>
@@ -7845,7 +7878,9 @@
       <c r="CE70" s="7">
         <v>0</v>
       </c>
-      <c r="CF70" s="8"/>
+      <c r="CF70" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="CG70" s="8">
         <v>4</v>
       </c>
@@ -7859,7 +7894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:89" ht="15.75" customHeight="1">
       <c r="B71" s="1" t="s">
         <v>16</v>
       </c>
@@ -8067,7 +8102,9 @@
       <c r="CE71" s="7">
         <v>-3000</v>
       </c>
-      <c r="CF71" s="8"/>
+      <c r="CF71" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="CG71" s="8">
         <v>0</v>
       </c>
@@ -8080,8 +8117,11 @@
       <c r="CJ71" s="8">
         <v>0</v>
       </c>
+      <c r="CK71" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="72" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:89" ht="15.75" customHeight="1">
       <c r="B72" s="1" t="s">
         <v>17</v>
       </c>
@@ -8289,7 +8329,9 @@
       <c r="CE72" s="7">
         <v>-2000</v>
       </c>
-      <c r="CF72" s="8"/>
+      <c r="CF72" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="CG72" s="8">
         <v>4</v>
       </c>
@@ -8303,7 +8345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:89" ht="15.75" customHeight="1">
       <c r="B73" s="1" t="s">
         <v>18</v>
       </c>
@@ -8511,7 +8553,9 @@
       <c r="CE73" s="7">
         <v>-16000</v>
       </c>
-      <c r="CF73" s="8"/>
+      <c r="CF73" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="CG73" s="8">
         <v>18</v>
       </c>
@@ -8528,7 +8572,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:89" ht="15.75" customHeight="1">
       <c r="B74" s="1" t="s">
         <v>19</v>
       </c>
@@ -8736,7 +8780,9 @@
       <c r="CE74" s="7">
         <v>0</v>
       </c>
-      <c r="CF74" s="8"/>
+      <c r="CF74" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="CG74" s="8">
         <v>0</v>
       </c>
@@ -8750,7 +8796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:89" ht="15.75" customHeight="1">
       <c r="B75" s="1" t="s">
         <v>20</v>
       </c>
@@ -8958,7 +9004,9 @@
       <c r="CE75" s="7">
         <v>13</v>
       </c>
-      <c r="CF75" s="8"/>
+      <c r="CF75" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="CG75" s="8">
         <v>1</v>
       </c>
@@ -8972,7 +9020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:89" ht="15.75" customHeight="1">
       <c r="B76" s="1" t="s">
         <v>21</v>
       </c>
@@ -9180,7 +9228,9 @@
       <c r="CE76" s="7">
         <v>0</v>
       </c>
-      <c r="CF76" s="8"/>
+      <c r="CF76" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="CG76" s="8">
         <v>3</v>
       </c>
@@ -9194,7 +9244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:89" ht="15.75" customHeight="1">
       <c r="B77" s="1" t="s">
         <v>22</v>
       </c>
@@ -9402,7 +9452,9 @@
       <c r="CE77" s="7">
         <v>0</v>
       </c>
-      <c r="CF77" s="8"/>
+      <c r="CF77" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="CG77" s="8">
         <v>-50000</v>
       </c>
@@ -9416,7 +9468,7 @@
         <v>-100000</v>
       </c>
     </row>
-    <row r="78" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:89" ht="15.75" customHeight="1">
       <c r="B78" s="1" t="s">
         <v>133</v>
       </c>
@@ -9624,7 +9676,9 @@
       <c r="CE78" s="7">
         <v>2</v>
       </c>
-      <c r="CF78" s="8"/>
+      <c r="CF78" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="CG78" s="8">
         <v>4</v>
       </c>
@@ -9638,7 +9692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:89" ht="15.75" customHeight="1">
       <c r="B79" s="1" t="s">
         <v>24</v>
       </c>
@@ -9846,7 +9900,9 @@
       <c r="CE79" s="7">
         <v>0</v>
       </c>
-      <c r="CF79" s="8"/>
+      <c r="CF79" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="CG79" s="8">
         <v>6</v>
       </c>
@@ -9860,7 +9916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="2:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:89" ht="15.75" customHeight="1">
       <c r="B80" s="1" t="s">
         <v>25</v>
       </c>
@@ -10068,7 +10124,9 @@
       <c r="CE80" s="7">
         <v>1</v>
       </c>
-      <c r="CF80" s="8"/>
+      <c r="CF80" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="CG80" s="8">
         <v>2</v>
       </c>
@@ -10082,7 +10140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:88" ht="15.75" customHeight="1">
       <c r="B81" s="1" t="s">
         <v>134</v>
       </c>
@@ -10290,7 +10348,9 @@
       <c r="CE81" s="7">
         <v>2</v>
       </c>
-      <c r="CF81" s="8"/>
+      <c r="CF81" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="CG81" s="8">
         <v>3</v>
       </c>
@@ -10304,7 +10364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:88" ht="15.75" customHeight="1">
       <c r="B82" s="1" t="s">
         <v>135</v>
       </c>
@@ -10512,7 +10572,9 @@
       <c r="CE82" s="7">
         <v>2</v>
       </c>
-      <c r="CF82" s="8"/>
+      <c r="CF82" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="CG82" s="8">
         <v>2</v>
       </c>
@@ -10526,7 +10588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:88" ht="15.75" customHeight="1">
       <c r="B83" s="1" t="s">
         <v>136</v>
       </c>
@@ -10734,7 +10796,9 @@
       <c r="CE83" s="7">
         <v>1</v>
       </c>
-      <c r="CF83" s="8"/>
+      <c r="CF83" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="CG83" s="8">
         <v>4</v>
       </c>
@@ -10748,7 +10812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:88" ht="15.75" customHeight="1">
       <c r="B84" s="1" t="s">
         <v>137</v>
       </c>
@@ -10956,7 +11020,9 @@
       <c r="CE84" s="7">
         <v>2</v>
       </c>
-      <c r="CF84" s="8"/>
+      <c r="CF84" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="CG84" s="8">
         <v>1</v>
       </c>
@@ -10970,7 +11036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:88" ht="15.75" customHeight="1">
       <c r="B85" s="1" t="s">
         <v>30</v>
       </c>
@@ -11178,7 +11244,9 @@
       <c r="CE85" s="7">
         <v>1</v>
       </c>
-      <c r="CF85" s="8"/>
+      <c r="CF85" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="CG85" s="8">
         <v>2</v>
       </c>
@@ -11192,7 +11260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:88" ht="15.75" customHeight="1">
       <c r="B86" s="1" t="s">
         <v>138</v>
       </c>
@@ -11400,7 +11468,9 @@
       <c r="CE86" s="7">
         <v>1</v>
       </c>
-      <c r="CF86" s="8"/>
+      <c r="CF86" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="CG86" s="8">
         <v>4</v>
       </c>
@@ -11414,7 +11484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:88" ht="15.75" customHeight="1">
       <c r="B87" s="1" t="s">
         <v>139</v>
       </c>
@@ -11622,7 +11692,9 @@
       <c r="CE87" s="7">
         <v>2</v>
       </c>
-      <c r="CF87" s="8"/>
+      <c r="CF87" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="CG87" s="8">
         <v>3</v>
       </c>
@@ -11636,7 +11708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:88" ht="15.75" customHeight="1">
       <c r="B88" s="1" t="s">
         <v>33</v>
       </c>
@@ -11844,7 +11916,9 @@
       <c r="CE88" s="7">
         <v>1</v>
       </c>
-      <c r="CF88" s="8"/>
+      <c r="CF88" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="CG88" s="8">
         <v>4</v>
       </c>
@@ -11858,7 +11932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:88" ht="15.75" customHeight="1">
       <c r="B89" s="1" t="s">
         <v>34</v>
       </c>
@@ -12066,7 +12140,9 @@
       <c r="CE89" s="7">
         <v>-8000</v>
       </c>
-      <c r="CF89" s="8"/>
+      <c r="CF89" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="CG89" s="8">
         <v>1</v>
       </c>
@@ -12080,7 +12156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:88" ht="15.75" customHeight="1">
       <c r="B90" s="1" t="s">
         <v>35</v>
       </c>
@@ -12288,7 +12364,9 @@
       <c r="CE90" s="7">
         <v>-9000</v>
       </c>
-      <c r="CF90" s="8"/>
+      <c r="CF90" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="CG90" s="8">
         <v>0</v>
       </c>
@@ -12302,7 +12380,7 @@
         <v>-90000</v>
       </c>
     </row>
-    <row r="91" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:88" ht="15.75" customHeight="1">
       <c r="B91" s="1" t="s">
         <v>36</v>
       </c>
@@ -12325,7 +12403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="2:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:88" ht="15.75" customHeight="1">
       <c r="CF92" t="s">
         <v>141</v>
       </c>
@@ -12342,7 +12420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="2:88" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:88">
       <c r="CF93" t="s">
         <v>142</v>
       </c>
@@ -12359,7 +12437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="2:88" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:88">
       <c r="CF94" t="s">
         <v>143</v>
       </c>
@@ -12377,7 +12455,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F54:CJ90 F93:CE96 CF91:CJ94">
+  <conditionalFormatting sqref="CF91:CJ94 F93:CE96 F54:CE90 CG54:CJ90">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
       <formula>6</formula>
       <formula>9</formula>
@@ -12391,6 +12469,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Write book stack part
</commit_message>
<xml_diff>
--- a/results/Random Sequences Results.xlsx
+++ b/results/Random Sequences Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
@@ -9,8 +9,9 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="144">
   <si>
     <t>BookStackTest_8dim_16up</t>
   </si>
@@ -203,12 +204,6 @@
   </si>
   <si>
     <t>Число Пи</t>
-  </si>
-  <si>
-    <t>Из 50</t>
-  </si>
-  <si>
-    <t>Из 10</t>
   </si>
   <si>
     <t>10000_Kbits</t>
@@ -463,8 +458,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -750,6 +745,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -784,6 +780,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -959,27 +956,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:DQ94"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" topLeftCell="E51" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="CE54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AV63" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E51" sqref="E51"/>
       <selection pane="topRight" activeCell="BT51" sqref="BT51"/>
       <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
-      <selection pane="bottomRight" activeCell="CF54" sqref="CF54:CJ90"/>
+      <selection pane="bottomRight" activeCell="AW61" sqref="AW61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="12.28515625"/>
     <col min="5" max="5" width="34.7109375" customWidth="1"/>
     <col min="6" max="83" width="12.28515625"/>
     <col min="84" max="84" width="21.140625"/>
-    <col min="85" max="1025" width="12.28515625"/>
+    <col min="85" max="86" width="12.42578125" customWidth="1"/>
+    <col min="89" max="1025" width="12.28515625"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:48" ht="15.75" customHeight="1">
+    <row r="4" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1103,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:48" ht="15.75" customHeight="1">
+    <row r="5" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1234,7 +1232,7 @@
         <v>-100000</v>
       </c>
     </row>
-    <row r="6" spans="2:48" ht="15.75" customHeight="1">
+    <row r="6" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1358,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:48" ht="15.75" customHeight="1">
+    <row r="7" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1489,7 +1487,7 @@
         <v>-89000</v>
       </c>
     </row>
-    <row r="8" spans="2:48" ht="15.75" customHeight="1">
+    <row r="8" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1613,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:48" ht="15.75" customHeight="1">
+    <row r="9" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1744,7 +1742,7 @@
         <v>-56000</v>
       </c>
     </row>
-    <row r="10" spans="2:48" ht="15.75" customHeight="1">
+    <row r="10" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1870,7 +1868,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:48" ht="15.75" customHeight="1">
+    <row r="11" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1999,7 +1997,7 @@
         <v>-51000</v>
       </c>
     </row>
-    <row r="12" spans="2:48" ht="15.75" customHeight="1">
+    <row r="12" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
@@ -2013,7 +2011,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="2:48" ht="15.75" customHeight="1">
+    <row r="13" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2029,7 +2027,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="2:48" ht="15.75" customHeight="1">
+    <row r="14" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2045,7 +2043,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="2:48" ht="15.75" customHeight="1">
+    <row r="15" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2061,7 +2059,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="2:48" ht="15.75" customHeight="1">
+    <row r="16" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2077,7 +2075,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="2:16" ht="15.75" customHeight="1">
+    <row r="17" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2093,7 +2091,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="2:16" ht="15.75" customHeight="1">
+    <row r="18" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2109,7 +2107,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" ht="15.75" customHeight="1">
+    <row r="19" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2125,7 +2123,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:16" ht="15.75" customHeight="1">
+    <row r="20" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2141,7 +2139,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="2:16" ht="15.75" customHeight="1">
+    <row r="21" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2157,7 +2155,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:16" ht="15.75" customHeight="1">
+    <row r="22" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2173,7 +2171,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:16" ht="15.75" customHeight="1">
+    <row r="23" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2189,7 +2187,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:16" ht="15.75" customHeight="1">
+    <row r="24" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2205,7 +2203,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:16" ht="15.75" customHeight="1">
+    <row r="25" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2221,7 +2219,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="2:16" ht="15.75" customHeight="1">
+    <row r="26" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2237,7 +2235,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="2:16" ht="15.75" customHeight="1">
+    <row r="27" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2253,7 +2251,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="2:16" ht="15.75" customHeight="1">
+    <row r="28" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2269,7 +2267,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="2:16" ht="15.75" customHeight="1">
+    <row r="29" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2285,7 +2283,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="2:16" ht="15.75" customHeight="1">
+    <row r="30" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2301,7 +2299,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="2:16" ht="15.75" customHeight="1">
+    <row r="31" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2317,7 +2315,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="2:16" ht="15.75" customHeight="1">
+    <row r="32" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2333,7 +2331,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="2:116" ht="15.75" customHeight="1">
+    <row r="33" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2349,7 +2347,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="2:116" ht="15.75" customHeight="1">
+    <row r="34" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2365,7 +2363,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="2:116" ht="15.75" customHeight="1">
+    <row r="35" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2427,7 +2425,7 @@
       <c r="BR35" s="1"/>
       <c r="BS35" s="1"/>
     </row>
-    <row r="36" spans="2:116" ht="15.75" customHeight="1">
+    <row r="36" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2489,7 +2487,7 @@
       <c r="BR36" s="1"/>
       <c r="BS36" s="1"/>
     </row>
-    <row r="37" spans="2:116" ht="15.75" customHeight="1">
+    <row r="37" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2551,7 +2549,7 @@
       <c r="BR37" s="1"/>
       <c r="BS37" s="1"/>
     </row>
-    <row r="38" spans="2:116" ht="15.75" customHeight="1">
+    <row r="38" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2619,7 +2617,7 @@
       <c r="BR38" s="1"/>
       <c r="BS38" s="1"/>
     </row>
-    <row r="39" spans="2:116" ht="15.75" customHeight="1">
+    <row r="39" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2682,7 +2680,7 @@
       <c r="BM39" s="1"/>
       <c r="BN39" s="1"/>
     </row>
-    <row r="40" spans="2:116" ht="15.75" customHeight="1">
+    <row r="40" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2745,7 +2743,7 @@
       <c r="BM40" s="1"/>
       <c r="BN40" s="1"/>
     </row>
-    <row r="41" spans="2:116" ht="15.75" customHeight="1">
+    <row r="41" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2825,9 +2823,8 @@
       <c r="CD41" s="1"/>
       <c r="CE41" s="1"/>
       <c r="CF41" s="1"/>
-      <c r="CG41" s="1"/>
     </row>
-    <row r="42" spans="2:116" ht="15.75" customHeight="1">
+    <row r="42" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2886,9 +2883,8 @@
       <c r="CD42" s="1"/>
       <c r="CE42" s="1"/>
       <c r="CF42" s="1"/>
-      <c r="CG42" s="1"/>
     </row>
-    <row r="43" spans="2:116" ht="15.75" customHeight="1">
+    <row r="43" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2971,9 +2967,8 @@
       <c r="CD43" s="1"/>
       <c r="CE43" s="1"/>
       <c r="CF43" s="1"/>
-      <c r="CG43" s="1"/>
     </row>
-    <row r="44" spans="2:116" ht="15.75" customHeight="1">
+    <row r="44" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -3058,8 +3053,6 @@
       <c r="CF44" s="1"/>
       <c r="CG44" s="1"/>
       <c r="CH44" s="1"/>
-      <c r="CI44" s="1"/>
-      <c r="CJ44" s="1"/>
       <c r="CK44" s="1"/>
       <c r="CL44" s="1"/>
       <c r="CM44" s="1"/>
@@ -3079,7 +3072,7 @@
       <c r="DA44" s="1"/>
       <c r="DB44" s="1"/>
     </row>
-    <row r="45" spans="2:116" ht="15.75" customHeight="1">
+    <row r="45" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -3164,8 +3157,6 @@
       <c r="CF45" s="1"/>
       <c r="CG45" s="1"/>
       <c r="CH45" s="1"/>
-      <c r="CI45" s="1"/>
-      <c r="CJ45" s="1"/>
       <c r="CK45" s="1"/>
       <c r="CL45" s="1"/>
       <c r="CM45" s="1"/>
@@ -3185,7 +3176,7 @@
       <c r="DA45" s="1"/>
       <c r="DB45" s="1"/>
     </row>
-    <row r="46" spans="2:116" ht="15.75" customHeight="1">
+    <row r="46" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3270,8 +3261,6 @@
       <c r="CF46" s="1"/>
       <c r="CG46" s="1"/>
       <c r="CH46" s="1"/>
-      <c r="CI46" s="1"/>
-      <c r="CJ46" s="1"/>
       <c r="CK46" s="1"/>
       <c r="CL46" s="1"/>
       <c r="CM46" s="1"/>
@@ -3301,7 +3290,7 @@
       <c r="DK46" s="1"/>
       <c r="DL46" s="1"/>
     </row>
-    <row r="47" spans="2:116" ht="15.75" customHeight="1">
+    <row r="47" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -3369,8 +3358,6 @@
       <c r="CF47" s="1"/>
       <c r="CG47" s="1"/>
       <c r="CH47" s="1"/>
-      <c r="CI47" s="1"/>
-      <c r="CJ47" s="1"/>
       <c r="CK47" s="1"/>
       <c r="CL47" s="1"/>
       <c r="CM47" s="1"/>
@@ -3400,7 +3387,7 @@
       <c r="DK47" s="1"/>
       <c r="DL47" s="1"/>
     </row>
-    <row r="48" spans="2:116" ht="15.75" customHeight="1">
+    <row r="48" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -3469,8 +3456,6 @@
       <c r="CF48" s="1"/>
       <c r="CG48" s="1"/>
       <c r="CH48" s="1"/>
-      <c r="CI48" s="1"/>
-      <c r="CJ48" s="1"/>
       <c r="CK48" s="1"/>
       <c r="CL48" s="1"/>
       <c r="CM48" s="1"/>
@@ -3500,7 +3485,7 @@
       <c r="DK48" s="1"/>
       <c r="DL48" s="1"/>
     </row>
-    <row r="49" spans="2:121" ht="15.75" customHeight="1">
+    <row r="49" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -3576,8 +3561,6 @@
       <c r="CF49" s="1"/>
       <c r="CG49" s="1"/>
       <c r="CH49" s="1"/>
-      <c r="CI49" s="1"/>
-      <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="1"/>
       <c r="CM49" s="1"/>
@@ -3612,7 +3595,7 @@
       <c r="DP49" s="1"/>
       <c r="DQ49" s="1"/>
     </row>
-    <row r="50" spans="2:121" ht="15.75" customHeight="1">
+    <row r="50" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -3665,8 +3648,6 @@
       <c r="CF50" s="1"/>
       <c r="CG50" s="1"/>
       <c r="CH50" s="1"/>
-      <c r="CI50" s="1"/>
-      <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="1"/>
       <c r="CM50" s="1"/>
@@ -3692,7 +3673,7 @@
       <c r="DG50" s="1"/>
       <c r="DH50" s="1"/>
     </row>
-    <row r="51" spans="2:121" ht="15.75" customHeight="1">
+    <row r="51" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H51" s="3" t="s">
         <v>41</v>
       </c>
@@ -3725,8 +3706,6 @@
       <c r="CF51" s="1"/>
       <c r="CG51" s="1"/>
       <c r="CH51" s="1"/>
-      <c r="CI51" s="1"/>
-      <c r="CJ51" s="1"/>
       <c r="CK51" s="1"/>
       <c r="CL51" s="1"/>
       <c r="CM51" s="1"/>
@@ -3756,7 +3735,7 @@
       <c r="DK51" s="1"/>
       <c r="DL51" s="1"/>
     </row>
-    <row r="52" spans="2:121" ht="15.75" customHeight="1">
+    <row r="52" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>43</v>
       </c>
@@ -3850,24 +3829,18 @@
         <v>60</v>
       </c>
       <c r="CG52" t="s">
+        <v>47</v>
+      </c>
+      <c r="CH52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="CH52" t="s">
+      <c r="E53" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="CI52" t="s">
-        <v>47</v>
-      </c>
-      <c r="CJ52" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="2:121" ht="15.75" customHeight="1">
-      <c r="C53" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>45</v>
@@ -3885,233 +3858,227 @@
         <v>40</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L53" s="6"/>
       <c r="M53" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N53" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O53" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N53" s="2" t="s">
+      <c r="P53" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="O53" s="2" t="s">
+      <c r="Q53" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="P53" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q53" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="R53" s="1" t="s">
         <v>50</v>
       </c>
       <c r="S53" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U53" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="T53" s="1" t="s">
+      <c r="V53" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="U53" s="1" t="s">
+      <c r="W53" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="V53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="W53" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="X53" s="1" t="s">
         <v>51</v>
       </c>
       <c r="Y53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA53" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="Z53" s="1" t="s">
+      <c r="AB53" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AA53" s="1" t="s">
+      <c r="AC53" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AB53" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC53" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="AD53" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AE53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF53" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG53" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AF53" s="1" t="s">
+      <c r="AH53" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AG53" s="1" t="s">
+      <c r="AI53" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AH53" s="1" t="s">
+      <c r="AJ53" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AI53" s="1" t="s">
+      <c r="AK53" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AJ53" s="1" t="s">
+      <c r="AL53" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AK53" s="1" t="s">
+      <c r="AM53" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AL53" s="1" t="s">
+      <c r="AN53" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AM53" s="1" t="s">
+      <c r="AO53" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="AN53" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AO53" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="AP53" s="1" t="s">
         <v>53</v>
       </c>
       <c r="AQ53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS53" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AR53" s="1" t="s">
+      <c r="AT53" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AS53" s="1" t="s">
+      <c r="AU53" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AT53" s="1" t="s">
+      <c r="AV53" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AU53" s="1" t="s">
+      <c r="AW53" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AV53" s="1" t="s">
+      <c r="AX53" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AW53" s="1" t="s">
+      <c r="AY53" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AX53" s="1" t="s">
+      <c r="AZ53" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AY53" s="1" t="s">
+      <c r="BA53" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="AZ53" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BA53" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="BB53" s="1" t="s">
         <v>55</v>
       </c>
       <c r="BC53" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BD53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BE53" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BD53" s="1" t="s">
+      <c r="BF53" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BE53" s="1" t="s">
+      <c r="BG53" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="BF53" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BG53" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="BH53" s="1" t="s">
         <v>56</v>
       </c>
       <c r="BI53" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BJ53" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BK53" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="BJ53" s="1" t="s">
+      <c r="BL53" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BK53" s="1" t="s">
+      <c r="BM53" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="BL53" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BM53" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="BN53" s="1" t="s">
         <v>57</v>
       </c>
       <c r="BO53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BP53" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BQ53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BP53" s="1" t="s">
+      <c r="BR53" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BQ53" s="1" t="s">
+      <c r="BS53" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="BR53" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="BS53" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="BT53" s="1" t="s">
         <v>58</v>
       </c>
       <c r="BU53" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BV53" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BW53" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BV53" s="1" t="s">
+      <c r="BX53" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BW53" s="1" t="s">
+      <c r="BY53" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="BX53" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="BY53" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="BZ53" s="1" t="s">
         <v>59</v>
       </c>
       <c r="CA53" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CB53" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="CC53" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="CB53" s="1" t="s">
+      <c r="CD53" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="CC53" s="1" t="s">
+      <c r="CE53" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="CD53" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="CE53" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="CG53" t="s">
         <v>38</v>
       </c>
       <c r="CH53" t="s">
         <v>40</v>
-      </c>
-      <c r="CI53" t="s">
-        <v>40</v>
-      </c>
-      <c r="CJ53" t="s">
-        <v>38</v>
       </c>
       <c r="CO53" s="1"/>
       <c r="CP53" s="1"/>
@@ -4128,7 +4095,7 @@
       <c r="DA53" s="1"/>
       <c r="DB53" s="1"/>
     </row>
-    <row r="54" spans="2:121" ht="15.75" customHeight="1">
+    <row r="54" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>0</v>
       </c>
@@ -4336,23 +4303,15 @@
       <c r="CE54" s="7">
         <v>1</v>
       </c>
-      <c r="CF54" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="CF54" s="1"/>
       <c r="CG54" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CH54" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI54" s="8">
-        <v>7</v>
-      </c>
-      <c r="CJ54" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="55" spans="2:121" ht="15.75" customHeight="1">
+    <row r="55" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>1</v>
       </c>
@@ -4456,16 +4415,14 @@
       </c>
       <c r="AP55" s="7"/>
       <c r="AQ55" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AR55" s="7"/>
       <c r="AS55" s="7"/>
       <c r="AT55" s="7"/>
       <c r="AU55" s="7"/>
       <c r="AV55" s="8"/>
-      <c r="AW55" s="7">
-        <v>19</v>
-      </c>
+      <c r="AW55" s="7"/>
       <c r="AX55" s="7">
         <v>3</v>
       </c>
@@ -4550,23 +4507,15 @@
       <c r="CE55" s="7">
         <v>1</v>
       </c>
-      <c r="CF55" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="CF55" s="1"/>
       <c r="CG55" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="CH55" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI55" s="8">
-        <v>5</v>
-      </c>
-      <c r="CJ55" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="2:121" ht="15.75" customHeight="1">
+    <row r="56" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
         <v>2</v>
       </c>
@@ -4679,15 +4628,9 @@
       <c r="AT56" s="7"/>
       <c r="AU56" s="7"/>
       <c r="AV56" s="8"/>
-      <c r="AW56" s="7">
-        <v>0</v>
-      </c>
-      <c r="AX56" s="7">
-        <v>0</v>
-      </c>
-      <c r="AY56" s="7">
-        <v>0</v>
-      </c>
+      <c r="AW56" s="7"/>
+      <c r="AX56" s="7"/>
+      <c r="AY56" s="7"/>
       <c r="AZ56" s="7">
         <v>0</v>
       </c>
@@ -4766,23 +4709,13 @@
       <c r="CE56" s="7">
         <v>0</v>
       </c>
-      <c r="CF56" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="CG56" s="8">
-        <v>0</v>
-      </c>
+      <c r="CF56" s="1"/>
+      <c r="CG56" s="8"/>
       <c r="CH56" s="8">
         <v>0</v>
       </c>
-      <c r="CI56" s="8">
-        <v>0</v>
-      </c>
-      <c r="CJ56" s="8">
-        <v>0</v>
-      </c>
     </row>
-    <row r="57" spans="2:121" ht="15.75" customHeight="1">
+    <row r="57" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
         <v>0</v>
       </c>
@@ -4990,23 +4923,15 @@
       <c r="CE57" s="7">
         <v>1</v>
       </c>
-      <c r="CF57" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="CF57" s="1"/>
       <c r="CG57" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CH57" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI57" s="8">
-        <v>7</v>
-      </c>
-      <c r="CJ57" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="58" spans="2:121" ht="15.75" customHeight="1">
+    <row r="58" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
         <v>3</v>
       </c>
@@ -5119,9 +5044,7 @@
       <c r="AT58" s="7"/>
       <c r="AU58" s="7"/>
       <c r="AV58" s="8"/>
-      <c r="AW58" s="7">
-        <v>5</v>
-      </c>
+      <c r="AW58" s="7"/>
       <c r="AX58" s="7">
         <v>8</v>
       </c>
@@ -5206,23 +5129,15 @@
       <c r="CE58" s="7">
         <v>1</v>
       </c>
-      <c r="CF58" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="CF58" s="1"/>
       <c r="CG58" s="8">
         <v>3</v>
       </c>
       <c r="CH58" s="8">
-        <v>2</v>
-      </c>
-      <c r="CI58" s="8">
-        <v>7</v>
-      </c>
-      <c r="CJ58" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="59" spans="2:121" ht="15.75" customHeight="1">
+    <row r="59" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>4</v>
       </c>
@@ -5335,15 +5250,9 @@
       <c r="AT59" s="7"/>
       <c r="AU59" s="7"/>
       <c r="AV59" s="8"/>
-      <c r="AW59" s="7">
-        <v>0</v>
-      </c>
-      <c r="AX59" s="7">
-        <v>8</v>
-      </c>
-      <c r="AY59" s="7">
-        <v>4</v>
-      </c>
+      <c r="AW59" s="7"/>
+      <c r="AX59" s="7"/>
+      <c r="AY59" s="7"/>
       <c r="AZ59" s="7">
         <v>9</v>
       </c>
@@ -5422,23 +5331,13 @@
       <c r="CE59" s="7">
         <v>0</v>
       </c>
-      <c r="CF59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="CG59" s="8">
-        <v>7</v>
-      </c>
+      <c r="CF59" s="1"/>
+      <c r="CG59" s="8"/>
       <c r="CH59" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI59" s="8">
         <v>8</v>
       </c>
-      <c r="CJ59" s="8">
-        <v>9</v>
-      </c>
     </row>
-    <row r="60" spans="2:121" ht="15.75" customHeight="1">
+    <row r="60" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
         <v>5</v>
       </c>
@@ -5646,31 +5545,23 @@
       <c r="CE60" s="7">
         <v>1</v>
       </c>
-      <c r="CF60" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="CF60" s="1"/>
       <c r="CG60" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="CH60" s="8">
-        <v>1</v>
-      </c>
-      <c r="CI60" s="8">
-        <v>3</v>
-      </c>
-      <c r="CJ60" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="61" spans="2:121" ht="15.75" customHeight="1">
+    <row r="61" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C61" s="1">
         <v>4</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="7">
@@ -5775,9 +5666,7 @@
       <c r="AT61" s="7"/>
       <c r="AU61" s="7"/>
       <c r="AV61" s="8"/>
-      <c r="AW61" s="7">
-        <v>9</v>
-      </c>
+      <c r="AW61" s="7"/>
       <c r="AX61" s="7">
         <v>7</v>
       </c>
@@ -5862,23 +5751,15 @@
       <c r="CE61" s="7">
         <v>0</v>
       </c>
-      <c r="CF61" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="CF61" s="1"/>
       <c r="CG61" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CH61" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI61" s="8">
-        <v>4</v>
-      </c>
-      <c r="CJ61" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="62" spans="2:121" ht="15.75" customHeight="1">
+    <row r="62" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
         <v>6</v>
       </c>
@@ -6086,23 +5967,15 @@
       <c r="CE62" s="7">
         <v>1</v>
       </c>
-      <c r="CF62" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="CF62" s="1"/>
       <c r="CG62" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="CH62" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI62" s="8">
-        <v>4</v>
-      </c>
-      <c r="CJ62" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="63" spans="2:121" ht="15.75" customHeight="1">
+    <row r="63" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
         <v>7</v>
       </c>
@@ -6310,25 +6183,17 @@
       <c r="CE63" s="7">
         <v>1</v>
       </c>
-      <c r="CF63" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="CF63" s="1"/>
       <c r="CG63" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH63" s="8">
         <v>0</v>
       </c>
-      <c r="CI63" s="8">
-        <v>0</v>
-      </c>
-      <c r="CJ63" s="8">
-        <v>1</v>
-      </c>
     </row>
-    <row r="64" spans="2:121" ht="15.75" customHeight="1">
+    <row r="64" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C64" s="1">
         <v>3</v>
@@ -6534,25 +6399,17 @@
       <c r="CE64" s="7">
         <v>1</v>
       </c>
-      <c r="CF64" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="CF64" s="1"/>
       <c r="CG64" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="CH64" s="8">
-        <v>1</v>
-      </c>
-      <c r="CI64" s="8">
-        <v>5</v>
-      </c>
-      <c r="CJ64" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:89" ht="15.75" customHeight="1">
+    <row r="65" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C65" s="1">
         <v>5</v>
@@ -6758,23 +6615,15 @@
       <c r="CE65" s="7">
         <v>0</v>
       </c>
-      <c r="CF65" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="CF65" s="1"/>
       <c r="CG65" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CH65" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI65" s="8">
-        <v>4</v>
-      </c>
-      <c r="CJ65" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="66" spans="2:89" ht="15.75" customHeight="1">
+    <row r="66" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
         <v>11</v>
       </c>
@@ -6798,7 +6647,7 @@
         <v>4</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L66" s="13"/>
       <c r="M66" s="8">
@@ -6982,23 +6831,15 @@
       <c r="CE66" s="7">
         <v>2</v>
       </c>
-      <c r="CF66" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="CF66" s="1"/>
       <c r="CG66" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="CH66" s="8">
-        <v>1</v>
-      </c>
-      <c r="CI66" s="8">
-        <v>6</v>
-      </c>
-      <c r="CJ66" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="67" spans="2:89" ht="15.75" customHeight="1">
+    <row r="67" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>12</v>
       </c>
@@ -7206,23 +7047,15 @@
       <c r="CE67" s="7">
         <v>2</v>
       </c>
-      <c r="CF67" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="CF67" s="1"/>
       <c r="CG67" s="8">
         <v>1</v>
       </c>
       <c r="CH67" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI67" s="8">
-        <v>6</v>
-      </c>
-      <c r="CJ67" s="8">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="68" spans="2:89" ht="15.75" customHeight="1">
+    <row r="68" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
         <v>13</v>
       </c>
@@ -7430,23 +7263,15 @@
       <c r="CE68" s="7">
         <v>0</v>
       </c>
-      <c r="CF68" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="CF68" s="1"/>
       <c r="CG68" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="CH68" s="8">
-        <v>1</v>
-      </c>
-      <c r="CI68" s="8">
-        <v>5</v>
-      </c>
-      <c r="CJ68" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="69" spans="2:89" ht="15.75" customHeight="1">
+    <row r="69" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
         <v>14</v>
       </c>
@@ -7654,23 +7479,15 @@
       <c r="CE69" s="7">
         <v>0</v>
       </c>
-      <c r="CF69" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="CF69" s="1"/>
       <c r="CG69" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="CH69" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI69" s="8">
-        <v>2</v>
-      </c>
-      <c r="CJ69" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="70" spans="2:89" ht="15.75" customHeight="1">
+    <row r="70" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
         <v>15</v>
       </c>
@@ -7878,23 +7695,15 @@
       <c r="CE70" s="7">
         <v>0</v>
       </c>
-      <c r="CF70" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="CF70" s="1"/>
       <c r="CG70" s="8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="CH70" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI70" s="8">
-        <v>5</v>
-      </c>
-      <c r="CJ70" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="71" spans="2:89" ht="15.75" customHeight="1">
+    <row r="71" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
         <v>16</v>
       </c>
@@ -8102,26 +7911,18 @@
       <c r="CE71" s="7">
         <v>-3000</v>
       </c>
-      <c r="CF71" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="CF71" s="1"/>
       <c r="CG71" s="8">
         <v>0</v>
       </c>
       <c r="CH71" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI71" s="8">
         <v>-2000</v>
       </c>
-      <c r="CJ71" s="8">
-        <v>0</v>
-      </c>
-      <c r="CK71" t="s">
-        <v>145</v>
+      <c r="CI71" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="72" spans="2:89" ht="15.75" customHeight="1">
+    <row r="72" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
         <v>17</v>
       </c>
@@ -8329,23 +8130,15 @@
       <c r="CE72" s="7">
         <v>-2000</v>
       </c>
-      <c r="CF72" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="CF72" s="1"/>
       <c r="CG72" s="8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="CH72" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI72" s="8">
         <v>9</v>
       </c>
-      <c r="CJ72" s="8">
-        <v>8</v>
-      </c>
     </row>
-    <row r="73" spans="2:89" ht="15.75" customHeight="1">
+    <row r="73" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
         <v>18</v>
       </c>
@@ -8553,26 +8346,18 @@
       <c r="CE73" s="7">
         <v>-16000</v>
       </c>
-      <c r="CF73" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="CF73" s="1"/>
       <c r="CG73" s="8">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="CH73" s="8">
-        <v>3</v>
-      </c>
-      <c r="CI73" s="8">
         <v>20</v>
       </c>
-      <c r="CJ73" s="8">
-        <v>25</v>
-      </c>
-      <c r="CK73" t="s">
-        <v>144</v>
+      <c r="CI73" t="s">
+        <v>142</v>
       </c>
     </row>
-    <row r="74" spans="2:89" ht="15.75" customHeight="1">
+    <row r="74" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
         <v>19</v>
       </c>
@@ -8780,23 +8565,15 @@
       <c r="CE74" s="7">
         <v>0</v>
       </c>
-      <c r="CF74" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="CF74" s="1"/>
       <c r="CG74" s="8">
         <v>0</v>
       </c>
       <c r="CH74" s="8">
         <v>0</v>
       </c>
-      <c r="CI74" s="8">
-        <v>0</v>
-      </c>
-      <c r="CJ74" s="8">
-        <v>0</v>
-      </c>
     </row>
-    <row r="75" spans="2:89" ht="15.75" customHeight="1">
+    <row r="75" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
         <v>20</v>
       </c>
@@ -9004,23 +8781,15 @@
       <c r="CE75" s="7">
         <v>13</v>
       </c>
-      <c r="CF75" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="CF75" s="1"/>
       <c r="CG75" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="CH75" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI75" s="8">
-        <v>4</v>
-      </c>
-      <c r="CJ75" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="2:89" ht="15.75" customHeight="1">
+    <row r="76" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
         <v>21</v>
       </c>
@@ -9228,23 +8997,15 @@
       <c r="CE76" s="7">
         <v>0</v>
       </c>
-      <c r="CF76" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="CF76" s="1"/>
       <c r="CG76" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="CH76" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI76" s="8">
-        <v>7</v>
-      </c>
-      <c r="CJ76" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="2:89" ht="15.75" customHeight="1">
+    <row r="77" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
         <v>22</v>
       </c>
@@ -9452,25 +9213,17 @@
       <c r="CE77" s="7">
         <v>0</v>
       </c>
-      <c r="CF77" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="CF77" s="1"/>
       <c r="CG77" s="8">
-        <v>-50000</v>
+        <v>-100000</v>
       </c>
       <c r="CH77" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI77" s="8">
-        <v>3</v>
-      </c>
-      <c r="CJ77" s="8">
-        <v>-100000</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:89" ht="15.75" customHeight="1">
+    <row r="78" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C78" s="1">
         <v>4</v>
@@ -9676,23 +9429,15 @@
       <c r="CE78" s="7">
         <v>2</v>
       </c>
-      <c r="CF78" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="CF78" s="1"/>
       <c r="CG78" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="CH78" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI78" s="8">
-        <v>5</v>
-      </c>
-      <c r="CJ78" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="79" spans="2:89" ht="15.75" customHeight="1">
+    <row r="79" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
         <v>24</v>
       </c>
@@ -9900,23 +9645,15 @@
       <c r="CE79" s="7">
         <v>0</v>
       </c>
-      <c r="CF79" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="CF79" s="1"/>
       <c r="CG79" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="CH79" s="8">
-        <v>1</v>
-      </c>
-      <c r="CI79" s="8">
-        <v>3</v>
-      </c>
-      <c r="CJ79" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="80" spans="2:89" ht="15.75" customHeight="1">
+    <row r="80" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
         <v>25</v>
       </c>
@@ -10124,25 +9861,17 @@
       <c r="CE80" s="7">
         <v>1</v>
       </c>
-      <c r="CF80" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="CF80" s="1"/>
       <c r="CG80" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="CH80" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI80" s="8">
-        <v>5</v>
-      </c>
-      <c r="CJ80" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="81" spans="2:88" ht="15.75" customHeight="1">
+    <row r="81" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C81" s="1">
         <v>5</v>
@@ -10348,25 +10077,17 @@
       <c r="CE81" s="7">
         <v>2</v>
       </c>
-      <c r="CF81" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="CF81" s="1"/>
       <c r="CG81" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="CH81" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI81" s="8">
-        <v>5</v>
-      </c>
-      <c r="CJ81" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="82" spans="2:88" ht="15.75" customHeight="1">
+    <row r="82" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C82" s="1">
         <v>8</v>
@@ -10572,25 +10293,17 @@
       <c r="CE82" s="7">
         <v>2</v>
       </c>
-      <c r="CF82" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="CF82" s="1"/>
       <c r="CG82" s="8">
         <v>2</v>
       </c>
       <c r="CH82" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI82" s="8">
-        <v>4</v>
-      </c>
-      <c r="CJ82" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="83" spans="2:88" ht="15.75" customHeight="1">
+    <row r="83" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C83" s="1">
         <v>2</v>
@@ -10796,25 +10509,17 @@
       <c r="CE83" s="7">
         <v>1</v>
       </c>
-      <c r="CF83" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="CF83" s="1"/>
       <c r="CG83" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="CH83" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI83" s="8">
-        <v>6</v>
-      </c>
-      <c r="CJ83" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="84" spans="2:88" ht="15.75" customHeight="1">
+    <row r="84" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C84" s="1">
         <v>2</v>
@@ -11020,23 +10725,15 @@
       <c r="CE84" s="7">
         <v>2</v>
       </c>
-      <c r="CF84" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="CF84" s="1"/>
       <c r="CG84" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CH84" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI84" s="8">
         <v>8</v>
       </c>
-      <c r="CJ84" s="8">
-        <v>2</v>
-      </c>
     </row>
-    <row r="85" spans="2:88" ht="15.75" customHeight="1">
+    <row r="85" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="s">
         <v>30</v>
       </c>
@@ -11244,25 +10941,17 @@
       <c r="CE85" s="7">
         <v>1</v>
       </c>
-      <c r="CF85" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="CF85" s="1"/>
       <c r="CG85" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="CH85" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI85" s="8">
-        <v>5</v>
-      </c>
-      <c r="CJ85" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="86" spans="2:88" ht="15.75" customHeight="1">
+    <row r="86" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C86" s="1">
         <v>5</v>
@@ -11468,25 +11157,17 @@
       <c r="CE86" s="7">
         <v>1</v>
       </c>
-      <c r="CF86" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="CF86" s="1"/>
       <c r="CG86" s="8">
         <v>4</v>
       </c>
       <c r="CH86" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI86" s="8">
-        <v>2</v>
-      </c>
-      <c r="CJ86" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="87" spans="2:88" ht="15.75" customHeight="1">
+    <row r="87" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C87" s="1">
         <v>100</v>
@@ -11692,23 +11373,15 @@
       <c r="CE87" s="7">
         <v>2</v>
       </c>
-      <c r="CF87" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="CF87" s="1"/>
       <c r="CG87" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="CH87" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI87" s="8">
-        <v>4</v>
-      </c>
-      <c r="CJ87" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="88" spans="2:88" ht="15.75" customHeight="1">
+    <row r="88" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="1" t="s">
         <v>33</v>
       </c>
@@ -11916,23 +11589,15 @@
       <c r="CE88" s="7">
         <v>1</v>
       </c>
-      <c r="CF88" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="CF88" s="1"/>
       <c r="CG88" s="8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="CH88" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI88" s="8">
-        <v>5</v>
-      </c>
-      <c r="CJ88" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="89" spans="2:88" ht="15.75" customHeight="1">
+    <row r="89" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="1" t="s">
         <v>34</v>
       </c>
@@ -12140,23 +11805,15 @@
       <c r="CE89" s="7">
         <v>-8000</v>
       </c>
-      <c r="CF89" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="CF89" s="1"/>
       <c r="CG89" s="8">
         <v>1</v>
       </c>
       <c r="CH89" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI89" s="8">
-        <v>7</v>
-      </c>
-      <c r="CJ89" s="8">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="90" spans="2:88" ht="15.75" customHeight="1">
+    <row r="90" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="s">
         <v>35</v>
       </c>
@@ -12364,23 +12021,15 @@
       <c r="CE90" s="7">
         <v>-9000</v>
       </c>
-      <c r="CF90" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="CF90" s="1"/>
       <c r="CG90" s="8">
-        <v>0</v>
+        <v>-90000</v>
       </c>
       <c r="CH90" s="8">
-        <v>0</v>
-      </c>
-      <c r="CI90" s="8">
-        <v>2</v>
-      </c>
-      <c r="CJ90" s="8">
-        <v>-90000</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="91" spans="2:88" ht="15.75" customHeight="1">
+    <row r="91" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="1" t="s">
         <v>36</v>
       </c>
@@ -12388,74 +12037,50 @@
         <v>-40000</v>
       </c>
       <c r="CF91" t="s">
+        <v>138</v>
+      </c>
+      <c r="CG91">
+        <v>4</v>
+      </c>
+      <c r="CH91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="CF92" t="s">
+        <v>139</v>
+      </c>
+      <c r="CG92">
+        <v>2</v>
+      </c>
+      <c r="CH92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="2:86" x14ac:dyDescent="0.2">
+      <c r="CF93" t="s">
         <v>140</v>
       </c>
-      <c r="CG91">
-        <v>2</v>
-      </c>
-      <c r="CH91">
-        <v>0</v>
-      </c>
-      <c r="CI91">
-        <v>2</v>
-      </c>
-      <c r="CJ91">
-        <v>4</v>
+      <c r="CG93">
+        <v>1</v>
+      </c>
+      <c r="CH93">
+        <v>6</v>
       </c>
     </row>
-    <row r="92" spans="2:88" ht="15.75" customHeight="1">
-      <c r="CF92" t="s">
+    <row r="94" spans="2:86" x14ac:dyDescent="0.2">
+      <c r="CF94" t="s">
         <v>141</v>
       </c>
-      <c r="CG92">
-        <v>1</v>
-      </c>
-      <c r="CH92">
-        <v>0</v>
-      </c>
-      <c r="CI92">
-        <v>8</v>
-      </c>
-      <c r="CJ92">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="2:88">
-      <c r="CF93" t="s">
-        <v>142</v>
-      </c>
-      <c r="CG93">
-        <v>1</v>
-      </c>
-      <c r="CH93">
-        <v>0</v>
-      </c>
-      <c r="CI93">
-        <v>6</v>
-      </c>
-      <c r="CJ93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="2:88">
-      <c r="CF94" t="s">
-        <v>143</v>
-      </c>
       <c r="CG94">
         <v>4</v>
       </c>
       <c r="CH94">
-        <v>0</v>
-      </c>
-      <c r="CI94">
-        <v>5</v>
-      </c>
-      <c r="CJ94">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="CF91:CJ94 F93:CE96 F54:CE90 CG54:CJ90">
+  <conditionalFormatting sqref="CF91:CF94 F93:CE96 F54:CE90 CG54:CH94">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
       <formula>6</formula>
       <formula>9</formula>
@@ -12471,4 +12096,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
STD gens description start
</commit_message>
<xml_diff>
--- a/results/Random Sequences Results.xlsx
+++ b/results/Random Sequences Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="178"/>
@@ -10,7 +10,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="148">
   <si>
     <t>BookStackTest_8dim_16up</t>
   </si>
@@ -458,16 +458,22 @@
   </si>
   <si>
     <t>ApproximateEntropy_2</t>
+  </si>
+  <si>
+    <t>mediana between std</t>
+  </si>
+  <si>
+    <t>mediana between all the gens</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -575,7 +581,260 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -728,7 +987,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -763,7 +1021,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -939,18 +1196,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:DQ94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E51" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="BZ54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="BE54" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E51" sqref="E51"/>
       <selection pane="topRight" activeCell="BT51" sqref="BT51"/>
       <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
-      <selection pane="bottomRight" activeCell="CF82" sqref="CF82"/>
+      <selection pane="bottomRight" activeCell="BI52" sqref="BI52:BM55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="4" width="12.140625"/>
     <col min="5" max="5" width="34.28515625"/>
@@ -961,7 +1218,7 @@
     <col min="89" max="1025" width="12.140625"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:48" ht="15.75" customHeight="1">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1344,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:48" ht="15.75" customHeight="1">
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1216,7 +1473,7 @@
         <v>-100000</v>
       </c>
     </row>
-    <row r="6" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:48" ht="15.75" customHeight="1">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1342,7 +1599,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:48" ht="15.75" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1471,7 +1728,7 @@
         <v>-89000</v>
       </c>
     </row>
-    <row r="8" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:48" ht="15.75" customHeight="1">
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1597,7 +1854,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:48" ht="15.75" customHeight="1">
       <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1726,7 +1983,7 @@
         <v>-56000</v>
       </c>
     </row>
-    <row r="10" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:48" ht="15.75" customHeight="1">
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1852,7 +2109,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:48" ht="15.75" customHeight="1">
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1981,7 +2238,7 @@
         <v>-51000</v>
       </c>
     </row>
-    <row r="12" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:48" ht="15.75" customHeight="1">
       <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1995,7 +2252,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:48" ht="15.75" customHeight="1">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2011,7 +2268,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:48" ht="15.75" customHeight="1">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2027,7 +2284,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:48" ht="15.75" customHeight="1">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2043,7 +2300,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="2:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:48" ht="15.75" customHeight="1">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2059,7 +2316,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:16" ht="15.75" customHeight="1">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2075,7 +2332,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:16" ht="15.75" customHeight="1">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2091,7 +2348,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:16" ht="15.75" customHeight="1">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2107,7 +2364,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:16" ht="15.75" customHeight="1">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2123,7 +2380,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:16" ht="15.75" customHeight="1">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2139,7 +2396,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:16" ht="15.75" customHeight="1">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2155,7 +2412,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" ht="15.75" customHeight="1">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2171,7 +2428,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" ht="15.75" customHeight="1">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2187,7 +2444,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" ht="15.75" customHeight="1">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2203,7 +2460,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" ht="15.75" customHeight="1">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2219,7 +2476,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" ht="15.75" customHeight="1">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2235,7 +2492,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" ht="15.75" customHeight="1">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2251,7 +2508,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" ht="15.75" customHeight="1">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2267,7 +2524,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:16" ht="15.75" customHeight="1">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2283,7 +2540,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:16" ht="15.75" customHeight="1">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2299,7 +2556,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:16" ht="15.75" customHeight="1">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2315,7 +2572,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:116" ht="15.75" customHeight="1">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2331,7 +2588,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:116" ht="15.75" customHeight="1">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2347,7 +2604,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:116" ht="15.75" customHeight="1">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2409,7 +2666,7 @@
       <c r="BR35" s="1"/>
       <c r="BS35" s="1"/>
     </row>
-    <row r="36" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:116" ht="15.75" customHeight="1">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2471,7 +2728,7 @@
       <c r="BR36" s="1"/>
       <c r="BS36" s="1"/>
     </row>
-    <row r="37" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:116" ht="15.75" customHeight="1">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2533,7 +2790,7 @@
       <c r="BR37" s="1"/>
       <c r="BS37" s="1"/>
     </row>
-    <row r="38" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:116" ht="15.75" customHeight="1">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2601,7 +2858,7 @@
       <c r="BR38" s="1"/>
       <c r="BS38" s="1"/>
     </row>
-    <row r="39" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:116" ht="15.75" customHeight="1">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2664,7 +2921,7 @@
       <c r="BM39" s="1"/>
       <c r="BN39" s="1"/>
     </row>
-    <row r="40" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:116" ht="15.75" customHeight="1">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2727,7 +2984,7 @@
       <c r="BM40" s="1"/>
       <c r="BN40" s="1"/>
     </row>
-    <row r="41" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:116" ht="15.75" customHeight="1">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2808,7 +3065,7 @@
       <c r="CE41" s="1"/>
       <c r="CF41" s="1"/>
     </row>
-    <row r="42" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:116" ht="15.75" customHeight="1">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2868,7 +3125,7 @@
       <c r="CE42" s="1"/>
       <c r="CF42" s="1"/>
     </row>
-    <row r="43" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:116" ht="15.75" customHeight="1">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2952,7 +3209,7 @@
       <c r="CE43" s="1"/>
       <c r="CF43" s="1"/>
     </row>
-    <row r="44" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:116" ht="15.75" customHeight="1">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -3056,7 +3313,7 @@
       <c r="DA44" s="1"/>
       <c r="DB44" s="1"/>
     </row>
-    <row r="45" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:116" ht="15.75" customHeight="1">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -3160,7 +3417,7 @@
       <c r="DA45" s="1"/>
       <c r="DB45" s="1"/>
     </row>
-    <row r="46" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:116" ht="15.75" customHeight="1">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3274,7 +3531,7 @@
       <c r="DK46" s="1"/>
       <c r="DL46" s="1"/>
     </row>
-    <row r="47" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:116" ht="15.75" customHeight="1">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -3371,7 +3628,7 @@
       <c r="DK47" s="1"/>
       <c r="DL47" s="1"/>
     </row>
-    <row r="48" spans="2:116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:116" ht="15.75" customHeight="1">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -3469,7 +3726,7 @@
       <c r="DK48" s="1"/>
       <c r="DL48" s="1"/>
     </row>
-    <row r="49" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:121" ht="15.75" customHeight="1">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -3579,7 +3836,7 @@
       <c r="DP49" s="1"/>
       <c r="DQ49" s="1"/>
     </row>
-    <row r="50" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:121" ht="15.75" customHeight="1">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -3657,7 +3914,7 @@
       <c r="DG50" s="1"/>
       <c r="DH50" s="1"/>
     </row>
-    <row r="51" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:121" ht="15.75" customHeight="1">
       <c r="H51" s="3" t="s">
         <v>41</v>
       </c>
@@ -3719,7 +3976,7 @@
       <c r="DK51" s="1"/>
       <c r="DL51" s="1"/>
     </row>
-    <row r="52" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:121" ht="15.75" customHeight="1">
       <c r="B52" s="1" t="s">
         <v>43</v>
       </c>
@@ -3733,12 +3990,8 @@
       <c r="H52" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I52" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
       <c r="K52" s="3" t="s">
         <v>47</v>
       </c>
@@ -3767,6 +4020,9 @@
       <c r="AI52" t="s">
         <v>49</v>
       </c>
+      <c r="AK52" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="AO52" t="s">
         <v>49</v>
       </c>
@@ -3776,6 +4032,9 @@
       <c r="AV52" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="AW52" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="BA52" t="s">
         <v>49</v>
       </c>
@@ -3819,7 +4078,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:121" ht="15.75" customHeight="1">
       <c r="C53" s="1" t="s">
         <v>61</v>
       </c>
@@ -4058,11 +4317,17 @@
       <c r="CE53" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="CF53" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="CG53" t="s">
         <v>38</v>
       </c>
       <c r="CH53" t="s">
         <v>40</v>
+      </c>
+      <c r="CJ53" t="s">
+        <v>146</v>
       </c>
       <c r="CO53" s="1"/>
       <c r="CP53" s="1"/>
@@ -4079,7 +4344,7 @@
       <c r="DA53" s="1"/>
       <c r="DB53" s="1"/>
     </row>
-    <row r="54" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:121" ht="15.75" customHeight="1">
       <c r="B54" s="1" t="s">
         <v>0</v>
       </c>
@@ -4297,8 +4562,12 @@
       <c r="CH54" s="8">
         <v>7</v>
       </c>
+      <c r="CJ54">
+        <f>AVERAGE(AW54:CE54)</f>
+        <v>4.9333333333333336</v>
+      </c>
     </row>
-    <row r="55" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:121" ht="15.75" customHeight="1">
       <c r="B55" s="1" t="s">
         <v>1</v>
       </c>
@@ -4502,8 +4771,12 @@
       <c r="CH55" s="8">
         <v>5</v>
       </c>
+      <c r="CJ55">
+        <f t="shared" ref="CJ55:CJ90" si="1">AVERAGE(AW55:CE55)</f>
+        <v>3.2916666666666665</v>
+      </c>
     </row>
-    <row r="56" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:121" ht="15.75" customHeight="1">
       <c r="B56" s="1" t="s">
         <v>2</v>
       </c>
@@ -4699,8 +4972,12 @@
       <c r="CH56" s="8">
         <v>0</v>
       </c>
+      <c r="CJ56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:121" ht="15.75" customHeight="1">
       <c r="B57" s="1" t="s">
         <v>0</v>
       </c>
@@ -4918,8 +5195,12 @@
       <c r="CH57" s="8">
         <v>7</v>
       </c>
+      <c r="CJ57">
+        <f t="shared" si="1"/>
+        <v>4.9333333333333336</v>
+      </c>
     </row>
-    <row r="58" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:121" ht="15.75" customHeight="1">
       <c r="B58" s="1" t="s">
         <v>3</v>
       </c>
@@ -5125,8 +5406,12 @@
       <c r="CH58" s="8">
         <v>7</v>
       </c>
+      <c r="CJ58">
+        <f t="shared" si="1"/>
+        <v>4.625</v>
+      </c>
     </row>
-    <row r="59" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:121" ht="15.75" customHeight="1">
       <c r="B59" s="1" t="s">
         <v>4</v>
       </c>
@@ -5322,8 +5607,12 @@
       <c r="CH59" s="8">
         <v>8</v>
       </c>
+      <c r="CJ59">
+        <f t="shared" si="1"/>
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="60" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:121" ht="15.75" customHeight="1">
       <c r="B60" s="1" t="s">
         <v>5</v>
       </c>
@@ -5541,8 +5830,12 @@
       <c r="CH60" s="8">
         <v>3</v>
       </c>
+      <c r="CJ60">
+        <f t="shared" si="1"/>
+        <v>4.5666666666666664</v>
+      </c>
     </row>
-    <row r="61" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:121" ht="15.75" customHeight="1">
       <c r="B61" s="1" t="s">
         <v>127</v>
       </c>
@@ -5739,7 +6032,7 @@
         <v>0</v>
       </c>
       <c r="CF61" s="14">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(G61:CE61)</f>
         <v>15.981481481481481</v>
       </c>
       <c r="CG61" s="8">
@@ -5748,8 +6041,12 @@
       <c r="CH61" s="8">
         <v>4</v>
       </c>
+      <c r="CJ61">
+        <f t="shared" si="1"/>
+        <v>4.166666666666667</v>
+      </c>
     </row>
-    <row r="62" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:121" ht="15.75" customHeight="1">
       <c r="B62" s="1" t="s">
         <v>6</v>
       </c>
@@ -5967,8 +6264,12 @@
       <c r="CH62" s="8">
         <v>4</v>
       </c>
+      <c r="CJ62">
+        <f t="shared" si="1"/>
+        <v>3.5666666666666669</v>
+      </c>
     </row>
-    <row r="63" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:121" ht="15.75" customHeight="1">
       <c r="B63" s="1" t="s">
         <v>7</v>
       </c>
@@ -6186,8 +6487,12 @@
       <c r="CH63" s="8">
         <v>0</v>
       </c>
+      <c r="CJ63">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="2:121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:121" ht="15.75" customHeight="1">
       <c r="B64" s="1" t="s">
         <v>128</v>
       </c>
@@ -6405,8 +6710,12 @@
       <c r="CH64" s="8">
         <v>5</v>
       </c>
+      <c r="CJ64">
+        <f t="shared" si="1"/>
+        <v>4.0333333333333332</v>
+      </c>
     </row>
-    <row r="65" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:88" ht="15.75" customHeight="1">
       <c r="B65" s="1" t="s">
         <v>129</v>
       </c>
@@ -6624,8 +6933,12 @@
       <c r="CH65" s="8">
         <v>4</v>
       </c>
+      <c r="CJ65">
+        <f t="shared" si="1"/>
+        <v>3.8</v>
+      </c>
     </row>
-    <row r="66" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:88" ht="15.75" customHeight="1">
       <c r="B66" s="1" t="s">
         <v>11</v>
       </c>
@@ -6843,8 +7156,12 @@
       <c r="CH66" s="8">
         <v>6</v>
       </c>
+      <c r="CJ66">
+        <f t="shared" si="1"/>
+        <v>4.166666666666667</v>
+      </c>
     </row>
-    <row r="67" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:88" ht="15.75" customHeight="1">
       <c r="B67" s="1" t="s">
         <v>12</v>
       </c>
@@ -7062,8 +7379,12 @@
       <c r="CH67" s="8">
         <v>6</v>
       </c>
+      <c r="CJ67">
+        <f t="shared" si="1"/>
+        <v>4.833333333333333</v>
+      </c>
     </row>
-    <row r="68" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:88" ht="15.75" customHeight="1">
       <c r="B68" s="1" t="s">
         <v>13</v>
       </c>
@@ -7281,8 +7602,12 @@
       <c r="CH68" s="8">
         <v>5</v>
       </c>
+      <c r="CJ68">
+        <f t="shared" si="1"/>
+        <v>5.0999999999999996</v>
+      </c>
     </row>
-    <row r="69" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:88" ht="15.75" customHeight="1">
       <c r="B69" s="1" t="s">
         <v>14</v>
       </c>
@@ -7500,8 +7825,12 @@
       <c r="CH69" s="8">
         <v>2</v>
       </c>
+      <c r="CJ69">
+        <f t="shared" si="1"/>
+        <v>4.2333333333333334</v>
+      </c>
     </row>
-    <row r="70" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:88" ht="15.75" customHeight="1">
       <c r="B70" s="1" t="s">
         <v>15</v>
       </c>
@@ -7719,8 +8048,12 @@
       <c r="CH70" s="8">
         <v>5</v>
       </c>
+      <c r="CJ70">
+        <f t="shared" si="1"/>
+        <v>4.7</v>
+      </c>
     </row>
-    <row r="71" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:88" ht="15.75" customHeight="1">
       <c r="B71" s="1" t="s">
         <v>16</v>
       </c>
@@ -7834,99 +8167,105 @@
       <c r="AU71" s="7"/>
       <c r="AV71" s="8"/>
       <c r="AW71" s="7">
-        <v>-8000</v>
+        <v>0</v>
       </c>
       <c r="AX71" s="7">
-        <v>-13000</v>
+        <v>0</v>
       </c>
       <c r="AY71" s="7">
-        <v>-11000</v>
+        <v>0</v>
       </c>
       <c r="AZ71" s="7">
-        <v>-4000</v>
+        <v>0</v>
       </c>
       <c r="BA71" s="7">
-        <v>-4000</v>
-      </c>
-      <c r="BB71" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="BB71" s="7">
+        <v>0</v>
+      </c>
       <c r="BC71" s="7">
-        <v>-11000</v>
+        <v>0</v>
       </c>
       <c r="BD71" s="7">
-        <v>-7000</v>
+        <v>0</v>
       </c>
       <c r="BE71" s="7">
-        <v>-8000</v>
+        <v>0</v>
       </c>
       <c r="BF71" s="7">
-        <v>-12000</v>
+        <v>0</v>
       </c>
       <c r="BG71" s="7">
-        <v>-1000</v>
-      </c>
-      <c r="BH71" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="BH71" s="7">
+        <v>0</v>
+      </c>
       <c r="BI71" s="7">
-        <v>-10000</v>
+        <v>0</v>
       </c>
       <c r="BJ71" s="7">
-        <v>-10000</v>
+        <v>0</v>
       </c>
       <c r="BK71" s="7">
-        <v>-16000</v>
+        <v>0</v>
       </c>
       <c r="BL71" s="7">
-        <v>-9000</v>
+        <v>0</v>
       </c>
       <c r="BM71" s="7">
-        <v>-2000</v>
-      </c>
-      <c r="BN71" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="BN71" s="7">
+        <v>0</v>
+      </c>
       <c r="BO71" s="7">
-        <v>-9000</v>
+        <v>0</v>
       </c>
       <c r="BP71" s="7">
-        <v>-12000</v>
+        <v>0</v>
       </c>
       <c r="BQ71" s="7">
-        <v>-13000</v>
+        <v>0</v>
       </c>
       <c r="BR71" s="7">
-        <v>-14000</v>
+        <v>0</v>
       </c>
       <c r="BS71" s="7">
-        <v>-3000</v>
-      </c>
-      <c r="BT71" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="BT71" s="7"/>
       <c r="BU71" s="7">
-        <v>-7000</v>
+        <v>0</v>
       </c>
       <c r="BV71" s="7">
-        <v>-10000</v>
+        <v>0</v>
       </c>
       <c r="BW71" s="7">
-        <v>-7000</v>
+        <v>0</v>
       </c>
       <c r="BX71" s="7">
-        <v>-6000</v>
+        <v>0</v>
       </c>
       <c r="BY71" s="7">
-        <v>-3000</v>
+        <v>0</v>
       </c>
       <c r="BZ71" s="7"/>
       <c r="CA71" s="7">
-        <v>-10000</v>
+        <v>0</v>
       </c>
       <c r="CB71" s="7">
-        <v>-11000</v>
+        <v>0</v>
       </c>
       <c r="CC71" s="7">
-        <v>-9000</v>
+        <v>0</v>
       </c>
       <c r="CD71" s="7">
-        <v>-7000</v>
+        <v>0</v>
       </c>
       <c r="CE71" s="7">
-        <v>-3000</v>
+        <v>0</v>
       </c>
       <c r="CF71" s="14"/>
       <c r="CG71" s="8">
@@ -7938,8 +8277,12 @@
       <c r="CI71" t="s">
         <v>131</v>
       </c>
+      <c r="CJ71">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="72" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:88" ht="15.75" customHeight="1">
       <c r="B72" s="1" t="s">
         <v>17</v>
       </c>
@@ -8053,99 +8396,105 @@
       <c r="AU72" s="7"/>
       <c r="AV72" s="8"/>
       <c r="AW72" s="7">
-        <v>-15000</v>
+        <v>0</v>
       </c>
       <c r="AX72" s="7">
-        <v>-15000</v>
+        <v>0</v>
       </c>
       <c r="AY72" s="7">
-        <v>-12000</v>
+        <v>0</v>
       </c>
       <c r="AZ72" s="7">
-        <v>-20000</v>
+        <v>0</v>
       </c>
       <c r="BA72" s="7">
-        <v>-3000</v>
-      </c>
-      <c r="BB72" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="BB72" s="7">
+        <v>0</v>
+      </c>
       <c r="BC72" s="7">
-        <v>-23000</v>
+        <v>0</v>
       </c>
       <c r="BD72" s="7">
-        <v>-18000</v>
+        <v>0</v>
       </c>
       <c r="BE72" s="7">
-        <v>-20000</v>
+        <v>0</v>
       </c>
       <c r="BF72" s="7">
-        <v>-16000</v>
+        <v>0</v>
       </c>
       <c r="BG72" s="7">
-        <v>-2000</v>
-      </c>
-      <c r="BH72" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="BH72" s="7">
+        <v>0</v>
+      </c>
       <c r="BI72" s="7">
-        <v>-13000</v>
+        <v>0</v>
       </c>
       <c r="BJ72" s="7">
-        <v>-17000</v>
+        <v>0</v>
       </c>
       <c r="BK72" s="7">
-        <v>-21000</v>
+        <v>0</v>
       </c>
       <c r="BL72" s="7">
-        <v>-15000</v>
+        <v>0</v>
       </c>
       <c r="BM72" s="7">
-        <v>-3000</v>
-      </c>
-      <c r="BN72" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="BN72" s="7">
+        <v>0</v>
+      </c>
       <c r="BO72" s="7">
-        <v>-17000</v>
+        <v>0</v>
       </c>
       <c r="BP72" s="7">
-        <v>-19000</v>
+        <v>0</v>
       </c>
       <c r="BQ72" s="7">
-        <v>-14000</v>
+        <v>0</v>
       </c>
       <c r="BR72" s="7">
-        <v>-19000</v>
+        <v>0</v>
       </c>
       <c r="BS72" s="7">
-        <v>-4000</v>
-      </c>
-      <c r="BT72" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="BT72" s="7"/>
       <c r="BU72" s="7">
-        <v>-16000</v>
+        <v>0</v>
       </c>
       <c r="BV72" s="7">
-        <v>-24000</v>
+        <v>0</v>
       </c>
       <c r="BW72" s="7">
-        <v>-18000</v>
+        <v>0</v>
       </c>
       <c r="BX72" s="7">
-        <v>-18000</v>
+        <v>0</v>
       </c>
       <c r="BY72" s="7">
-        <v>-2000</v>
+        <v>0</v>
       </c>
       <c r="BZ72" s="7"/>
       <c r="CA72" s="7">
-        <v>-24000</v>
+        <v>0</v>
       </c>
       <c r="CB72" s="7">
-        <v>-17000</v>
+        <v>0</v>
       </c>
       <c r="CC72" s="7">
-        <v>-16000</v>
+        <v>0</v>
       </c>
       <c r="CD72" s="7">
-        <v>-16000</v>
+        <v>0</v>
       </c>
       <c r="CE72" s="7">
-        <v>-2000</v>
+        <v>0</v>
       </c>
       <c r="CF72" s="14"/>
       <c r="CG72" s="8">
@@ -8154,8 +8503,12 @@
       <c r="CH72" s="8">
         <v>9</v>
       </c>
+      <c r="CJ72">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:88" ht="15.75" customHeight="1">
       <c r="B73" s="1" t="s">
         <v>18</v>
       </c>
@@ -8269,99 +8622,105 @@
       <c r="AU73" s="7"/>
       <c r="AV73" s="8"/>
       <c r="AW73" s="7">
-        <v>-59000</v>
+        <v>0</v>
       </c>
       <c r="AX73" s="7">
-        <v>-59000</v>
+        <v>0</v>
       </c>
       <c r="AY73" s="7">
-        <v>-57000</v>
+        <v>0</v>
       </c>
       <c r="AZ73" s="7">
-        <v>-46000</v>
+        <v>0</v>
       </c>
       <c r="BA73" s="7">
-        <v>-12000</v>
-      </c>
-      <c r="BB73" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="BB73" s="7">
+        <v>0</v>
+      </c>
       <c r="BC73" s="7">
-        <v>-58000</v>
+        <v>0</v>
       </c>
       <c r="BD73" s="7">
-        <v>-51000</v>
+        <v>0</v>
       </c>
       <c r="BE73" s="7">
-        <v>-56000</v>
+        <v>0</v>
       </c>
       <c r="BF73" s="7">
-        <v>-55000</v>
+        <v>0</v>
       </c>
       <c r="BG73" s="7">
-        <v>-10000</v>
-      </c>
-      <c r="BH73" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="BH73" s="7">
+        <v>0</v>
+      </c>
       <c r="BI73" s="7">
-        <v>-60000</v>
+        <v>0</v>
       </c>
       <c r="BJ73" s="7">
-        <v>-58000</v>
+        <v>0</v>
       </c>
       <c r="BK73" s="7">
-        <v>-62000</v>
+        <v>0</v>
       </c>
       <c r="BL73" s="7">
-        <v>-60000</v>
+        <v>0</v>
       </c>
       <c r="BM73" s="7">
-        <v>-15000</v>
-      </c>
-      <c r="BN73" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="BN73" s="7">
+        <v>0</v>
+      </c>
       <c r="BO73" s="7">
-        <v>-59000</v>
+        <v>0</v>
       </c>
       <c r="BP73" s="7">
-        <v>-57000</v>
+        <v>0</v>
       </c>
       <c r="BQ73" s="7">
-        <v>-60000</v>
+        <v>0</v>
       </c>
       <c r="BR73" s="7">
-        <v>-64000</v>
+        <v>0</v>
       </c>
       <c r="BS73" s="7">
-        <v>-14000</v>
-      </c>
-      <c r="BT73" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="BT73" s="7"/>
       <c r="BU73" s="7">
-        <v>-61000</v>
+        <v>0</v>
       </c>
       <c r="BV73" s="7">
-        <v>-54000</v>
+        <v>0</v>
       </c>
       <c r="BW73" s="7">
-        <v>-59000</v>
+        <v>0</v>
       </c>
       <c r="BX73" s="7">
-        <v>-54000</v>
+        <v>0</v>
       </c>
       <c r="BY73" s="7">
-        <v>-8000</v>
+        <v>0</v>
       </c>
       <c r="BZ73" s="7"/>
       <c r="CA73" s="7">
-        <v>-54000</v>
+        <v>0</v>
       </c>
       <c r="CB73" s="7">
-        <v>-53000</v>
+        <v>0</v>
       </c>
       <c r="CC73" s="7">
-        <v>-61000</v>
+        <v>0</v>
       </c>
       <c r="CD73" s="7">
-        <v>-63000</v>
+        <v>0</v>
       </c>
       <c r="CE73" s="7">
-        <v>-16000</v>
+        <v>0</v>
       </c>
       <c r="CF73" s="14"/>
       <c r="CG73" s="8">
@@ -8373,8 +8732,12 @@
       <c r="CI73" t="s">
         <v>132</v>
       </c>
+      <c r="CJ73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="74" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:88" ht="15.75" customHeight="1">
       <c r="B74" s="1" t="s">
         <v>19</v>
       </c>
@@ -8592,8 +8955,12 @@
       <c r="CH74" s="8">
         <v>0</v>
       </c>
+      <c r="CJ74">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="75" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:88" ht="15.75" customHeight="1">
       <c r="B75" s="1" t="s">
         <v>20</v>
       </c>
@@ -8813,8 +9180,12 @@
       <c r="CH75" s="8">
         <v>4</v>
       </c>
+      <c r="CJ75">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="76" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:88" ht="15.75" customHeight="1">
       <c r="B76" s="1" t="s">
         <v>21</v>
       </c>
@@ -8825,9 +9196,7 @@
         <v>20</v>
       </c>
       <c r="F76" s="1"/>
-      <c r="G76" s="7">
-        <v>23</v>
-      </c>
+      <c r="G76" s="7"/>
       <c r="H76" s="7">
         <v>7</v>
       </c>
@@ -8841,9 +9210,7 @@
         <v>6</v>
       </c>
       <c r="L76" s="7"/>
-      <c r="M76" s="8">
-        <v>14</v>
-      </c>
+      <c r="M76" s="8"/>
       <c r="N76" s="8">
         <v>8</v>
       </c>
@@ -8857,9 +9224,7 @@
         <v>1</v>
       </c>
       <c r="R76" s="7"/>
-      <c r="S76" s="7">
-        <v>35</v>
-      </c>
+      <c r="S76" s="7"/>
       <c r="T76" s="7">
         <v>34</v>
       </c>
@@ -8873,9 +9238,7 @@
         <v>14</v>
       </c>
       <c r="X76" s="7"/>
-      <c r="Y76" s="7">
-        <v>23</v>
-      </c>
+      <c r="Y76" s="7"/>
       <c r="Z76" s="7">
         <v>5</v>
       </c>
@@ -8889,9 +9252,7 @@
         <v>2</v>
       </c>
       <c r="AD76" s="7"/>
-      <c r="AE76" s="7">
-        <v>24</v>
-      </c>
+      <c r="AE76" s="7"/>
       <c r="AF76" s="7">
         <v>10</v>
       </c>
@@ -8905,9 +9266,7 @@
         <v>1</v>
       </c>
       <c r="AJ76" s="7"/>
-      <c r="AK76" s="7">
-        <v>17</v>
-      </c>
+      <c r="AK76" s="7"/>
       <c r="AL76" s="7">
         <v>5</v>
       </c>
@@ -8927,23 +9286,22 @@
       <c r="AT76" s="7"/>
       <c r="AU76" s="7"/>
       <c r="AV76" s="8"/>
-      <c r="AW76" s="7" t="s">
+      <c r="AX76" s="7">
+        <v>2</v>
+      </c>
+      <c r="AY76" s="7">
+        <v>4</v>
+      </c>
+      <c r="AZ76" s="7">
+        <v>3</v>
+      </c>
+      <c r="BA76" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB76" s="7"/>
+      <c r="BC76" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="AX76" s="7">
-        <v>2</v>
-      </c>
-      <c r="AY76" s="7">
-        <v>4</v>
-      </c>
-      <c r="AZ76" s="7">
-        <v>3</v>
-      </c>
-      <c r="BA76" s="7">
-        <v>1</v>
-      </c>
-      <c r="BB76" s="7"/>
-      <c r="BC76" s="7"/>
       <c r="BD76" s="7">
         <v>9</v>
       </c>
@@ -9014,7 +9372,7 @@
       </c>
       <c r="CF76" s="14">
         <f t="shared" si="0"/>
-        <v>8.0370370370370363</v>
+        <v>6.208333333333333</v>
       </c>
       <c r="CG76" s="8">
         <v>7</v>
@@ -9022,8 +9380,12 @@
       <c r="CH76" s="8">
         <v>7</v>
       </c>
+      <c r="CJ76">
+        <f>AVERAGE(AX76:CE76)</f>
+        <v>4.375</v>
+      </c>
     </row>
-    <row r="77" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:88" ht="15.75" customHeight="1">
       <c r="B77" s="1" t="s">
         <v>22</v>
       </c>
@@ -9197,8 +9559,12 @@
       <c r="CH77" s="8">
         <v>3</v>
       </c>
+      <c r="CJ77">
+        <f t="shared" si="1"/>
+        <v>4.3888888888888893</v>
+      </c>
     </row>
-    <row r="78" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:88" ht="15.75" customHeight="1">
       <c r="B78" s="1" t="s">
         <v>135</v>
       </c>
@@ -9416,8 +9782,12 @@
       <c r="CH78" s="8">
         <v>5</v>
       </c>
+      <c r="CJ78">
+        <f t="shared" si="1"/>
+        <v>4.5333333333333332</v>
+      </c>
     </row>
-    <row r="79" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:88" ht="15.75" customHeight="1">
       <c r="B79" s="1" t="s">
         <v>24</v>
       </c>
@@ -9635,8 +10005,12 @@
       <c r="CH79" s="8">
         <v>3</v>
       </c>
+      <c r="CJ79">
+        <f t="shared" si="1"/>
+        <v>3.8666666666666667</v>
+      </c>
     </row>
-    <row r="80" spans="2:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:88" ht="15.75" customHeight="1">
       <c r="B80" s="1" t="s">
         <v>25</v>
       </c>
@@ -9854,8 +10228,12 @@
       <c r="CH80" s="8">
         <v>5</v>
       </c>
+      <c r="CJ80">
+        <f t="shared" si="1"/>
+        <v>4.166666666666667</v>
+      </c>
     </row>
-    <row r="81" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:88" ht="15.75" customHeight="1">
       <c r="B81" s="1" t="s">
         <v>136</v>
       </c>
@@ -10073,8 +10451,12 @@
       <c r="CH81" s="8">
         <v>5</v>
       </c>
+      <c r="CJ81">
+        <f t="shared" si="1"/>
+        <v>3.8333333333333335</v>
+      </c>
     </row>
-    <row r="82" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:88" ht="15.75" customHeight="1">
       <c r="B82" s="1" t="s">
         <v>137</v>
       </c>
@@ -10280,8 +10662,12 @@
       <c r="CH82" s="8">
         <v>4</v>
       </c>
+      <c r="CJ82">
+        <f t="shared" si="1"/>
+        <v>3.7083333333333335</v>
+      </c>
     </row>
-    <row r="83" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:88" ht="15.75" customHeight="1">
       <c r="B83" s="1" t="s">
         <v>138</v>
       </c>
@@ -10487,8 +10873,12 @@
       <c r="CH83" s="8">
         <v>6</v>
       </c>
+      <c r="CJ83">
+        <f t="shared" si="1"/>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="84" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:88" ht="15.75" customHeight="1">
       <c r="B84" s="1" t="s">
         <v>139</v>
       </c>
@@ -10706,8 +11096,12 @@
       <c r="CH84" s="8">
         <v>8</v>
       </c>
+      <c r="CJ84">
+        <f t="shared" si="1"/>
+        <v>4.5666666666666664</v>
+      </c>
     </row>
-    <row r="85" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:88" ht="15.75" customHeight="1">
       <c r="B85" s="1" t="s">
         <v>30</v>
       </c>
@@ -10925,8 +11319,12 @@
       <c r="CH85" s="8">
         <v>5</v>
       </c>
+      <c r="CJ85">
+        <f t="shared" si="1"/>
+        <v>4.2333333333333334</v>
+      </c>
     </row>
-    <row r="86" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:88" ht="15.75" customHeight="1">
       <c r="B86" s="1" t="s">
         <v>140</v>
       </c>
@@ -11144,8 +11542,12 @@
       <c r="CH86" s="8">
         <v>2</v>
       </c>
+      <c r="CJ86">
+        <f t="shared" si="1"/>
+        <v>4.666666666666667</v>
+      </c>
     </row>
-    <row r="87" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:88" ht="15.75" customHeight="1">
       <c r="B87" s="1" t="s">
         <v>141</v>
       </c>
@@ -11363,8 +11765,12 @@
       <c r="CH87" s="8">
         <v>4</v>
       </c>
+      <c r="CJ87">
+        <f t="shared" si="1"/>
+        <v>3.8</v>
+      </c>
     </row>
-    <row r="88" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:88" ht="15.75" customHeight="1">
       <c r="B88" s="1" t="s">
         <v>33</v>
       </c>
@@ -11582,8 +11988,12 @@
       <c r="CH88" s="8">
         <v>5</v>
       </c>
+      <c r="CJ88">
+        <f t="shared" si="1"/>
+        <v>3.5666666666666669</v>
+      </c>
     </row>
-    <row r="89" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:88" ht="15.75" customHeight="1">
       <c r="B89" s="1" t="s">
         <v>34</v>
       </c>
@@ -11696,100 +12106,64 @@
       <c r="AT89" s="7"/>
       <c r="AU89" s="7"/>
       <c r="AV89" s="8"/>
-      <c r="AW89" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="AX89" s="7">
-        <v>-84000</v>
-      </c>
-      <c r="AY89" s="7">
-        <v>-52000</v>
-      </c>
+      <c r="AW89" s="7"/>
+      <c r="AX89" s="7"/>
+      <c r="AY89" s="7"/>
       <c r="AZ89" s="7">
-        <v>-43000</v>
+        <v>0</v>
       </c>
       <c r="BA89" s="7">
-        <v>-2000</v>
+        <v>0</v>
       </c>
       <c r="BB89" s="7"/>
-      <c r="BC89" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="BD89" s="7">
-        <v>-93000</v>
-      </c>
-      <c r="BE89" s="7">
-        <v>-57000</v>
-      </c>
+      <c r="BC89" s="7"/>
+      <c r="BD89" s="7"/>
+      <c r="BE89" s="7"/>
       <c r="BF89" s="7">
-        <v>-40000</v>
+        <v>0</v>
       </c>
       <c r="BG89" s="7">
-        <v>-3000</v>
+        <v>0</v>
       </c>
       <c r="BH89" s="7"/>
-      <c r="BI89" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="BJ89" s="7">
-        <v>-91000</v>
-      </c>
-      <c r="BK89" s="7">
-        <v>-50000</v>
-      </c>
+      <c r="BI89" s="7"/>
+      <c r="BJ89" s="7"/>
+      <c r="BK89" s="7"/>
       <c r="BL89" s="7">
-        <v>-35000</v>
+        <v>0</v>
       </c>
       <c r="BM89" s="7">
-        <v>-2000</v>
+        <v>0</v>
       </c>
       <c r="BN89" s="7"/>
-      <c r="BO89" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="BP89" s="7">
-        <v>-86000</v>
-      </c>
-      <c r="BQ89" s="7">
-        <v>-52000</v>
-      </c>
+      <c r="BO89" s="7"/>
+      <c r="BP89" s="7"/>
+      <c r="BQ89" s="7"/>
       <c r="BR89" s="7">
-        <v>-39000</v>
+        <v>0</v>
       </c>
       <c r="BS89" s="7">
-        <v>-3000</v>
+        <v>0</v>
       </c>
       <c r="BT89" s="8"/>
-      <c r="BU89" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="BV89" s="7">
-        <v>-90000</v>
-      </c>
-      <c r="BW89" s="7">
-        <v>-53000</v>
-      </c>
+      <c r="BU89" s="7"/>
+      <c r="BV89" s="7"/>
+      <c r="BW89" s="7"/>
       <c r="BX89" s="7">
-        <v>-40000</v>
+        <v>0</v>
       </c>
       <c r="BY89" s="7">
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="BZ89" s="7"/>
-      <c r="CA89" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="CB89" s="7">
-        <v>-93000</v>
-      </c>
-      <c r="CC89" s="7">
-        <v>-57000</v>
-      </c>
+      <c r="CA89" s="7"/>
+      <c r="CB89" s="7"/>
+      <c r="CC89" s="7"/>
       <c r="CD89" s="7">
-        <v>-40000</v>
+        <v>0</v>
       </c>
       <c r="CE89" s="7">
-        <v>-8000</v>
+        <v>0</v>
       </c>
       <c r="CF89" s="1"/>
       <c r="CG89" s="8">
@@ -11798,8 +12172,12 @@
       <c r="CH89" s="8">
         <v>7</v>
       </c>
+      <c r="CJ89">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="90" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:88" ht="15.75" customHeight="1">
       <c r="B90" s="1" t="s">
         <v>35</v>
       </c>
@@ -11912,100 +12290,64 @@
       <c r="AT90" s="7"/>
       <c r="AU90" s="7"/>
       <c r="AV90" s="8"/>
-      <c r="AW90" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="AX90" s="7">
-        <v>-85000</v>
-      </c>
-      <c r="AY90" s="7">
-        <v>-60000</v>
-      </c>
+      <c r="AW90" s="7"/>
+      <c r="AX90" s="7"/>
+      <c r="AY90" s="7"/>
       <c r="AZ90" s="7">
-        <v>-45000</v>
+        <v>0</v>
       </c>
       <c r="BA90" s="7">
-        <v>-4000</v>
+        <v>0</v>
       </c>
       <c r="BB90" s="7"/>
-      <c r="BC90" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="BD90" s="7">
-        <v>-95000</v>
-      </c>
-      <c r="BE90" s="7">
-        <v>-59000</v>
-      </c>
+      <c r="BC90" s="7"/>
+      <c r="BD90" s="7"/>
+      <c r="BE90" s="7"/>
       <c r="BF90" s="7">
-        <v>-53000</v>
+        <v>0</v>
       </c>
       <c r="BG90" s="7">
-        <v>-7000</v>
+        <v>0</v>
       </c>
       <c r="BH90" s="7"/>
-      <c r="BI90" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="BJ90" s="7">
-        <v>-93000</v>
-      </c>
-      <c r="BK90" s="7">
-        <v>-56000</v>
-      </c>
+      <c r="BI90" s="7"/>
+      <c r="BJ90" s="7"/>
+      <c r="BK90" s="7"/>
       <c r="BL90" s="7">
-        <v>-45000</v>
+        <v>0</v>
       </c>
       <c r="BM90" s="7">
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="BN90" s="7"/>
-      <c r="BO90" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="BP90" s="7">
-        <v>-87000</v>
-      </c>
-      <c r="BQ90" s="7">
-        <v>-60000</v>
-      </c>
+      <c r="BO90" s="7"/>
+      <c r="BP90" s="7"/>
+      <c r="BQ90" s="7"/>
       <c r="BR90" s="7">
-        <v>-46000</v>
+        <v>0</v>
       </c>
       <c r="BS90" s="7">
-        <v>-4000</v>
+        <v>0</v>
       </c>
       <c r="BT90" s="8"/>
-      <c r="BU90" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="BV90" s="7">
-        <v>-92000</v>
-      </c>
-      <c r="BW90" s="7">
-        <v>-57000</v>
-      </c>
+      <c r="BU90" s="7"/>
+      <c r="BV90" s="7"/>
+      <c r="BW90" s="7"/>
       <c r="BX90" s="7">
-        <v>-42000</v>
+        <v>0</v>
       </c>
       <c r="BY90" s="7">
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="BZ90" s="7"/>
-      <c r="CA90" s="7">
-        <v>-100000</v>
-      </c>
-      <c r="CB90" s="7">
-        <v>-92000</v>
-      </c>
-      <c r="CC90" s="7">
-        <v>-65000</v>
-      </c>
+      <c r="CA90" s="7"/>
+      <c r="CB90" s="7"/>
+      <c r="CC90" s="7"/>
       <c r="CD90" s="7">
-        <v>-48000</v>
+        <v>0</v>
       </c>
       <c r="CE90" s="7">
-        <v>-9000</v>
+        <v>0</v>
       </c>
       <c r="CF90" s="1"/>
       <c r="CG90" s="8">
@@ -12014,8 +12356,12 @@
       <c r="CH90" s="8">
         <v>2</v>
       </c>
+      <c r="CJ90">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="91" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:88" ht="15.75" customHeight="1">
       <c r="B91" s="1" t="s">
         <v>36</v>
       </c>
@@ -12032,7 +12378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="2:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:88" ht="15.75" customHeight="1">
       <c r="CF92" s="5" t="s">
         <v>143</v>
       </c>
@@ -12043,7 +12389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:88">
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
       <c r="H93" s="5"/>
@@ -12132,7 +12478,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="2:86" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:88">
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
@@ -12222,20 +12568,39 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="CF82">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
+      <formula>6</formula>
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CG54:CH94 G54:AV90 AW54:AW75 AW77:AW90 AX54:CE90">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>19</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>10</formula>
+      <formula>19</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+      <formula>6</formula>
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCellId="1" sqref="CA66 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1025" width="8.5703125"/>
   </cols>

</xml_diff>